<commit_message>
Rounded Bag with volumen and radius text
</commit_message>
<xml_diff>
--- a/static/files/Baglab_roundedCorners.xlsx
+++ b/static/files/Baglab_roundedCorners.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <workbookProtection lockWindows="false"/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Double U" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Cut Du" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Radius helper" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'Cut Du'!$A$1:$N$67</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Double U'!$A$1:$Q$42</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Double U'!$A$1:$Q$43</definedName>
     <definedName function="false" hidden="false" name="Br" vbProcedure="false">'Double U'!$C$7</definedName>
     <definedName function="false" hidden="false" name="Ho" vbProcedure="false">'Double U'!$C$8</definedName>
     <definedName function="false" hidden="false" name="Hs" vbProcedure="false">'Double U'!$C$9</definedName>
@@ -24,14 +25,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="94">
   <si>
     <t xml:space="preserve">ROUND</t>
   </si>
@@ -96,6 +97,9 @@
     <t xml:space="preserve">SegmenthöheH_s</t>
   </si>
   <si>
+    <t xml:space="preserve">Volumen</t>
+  </si>
+  <si>
     <t xml:space="preserve">U / 8</t>
   </si>
   <si>
@@ -295,24 +299,39 @@
   </si>
   <si>
     <t xml:space="preserve">siehe obrn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What </t>
+  </si>
+  <si>
+    <t xml:space="preserve">diamter </t>
+  </si>
+  <si>
+    <t xml:space="preserve">radius excl 1cm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0\ [$cm ]"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00\ [$€-407];[RED]\-#,##0.00\ [$€-407]"/>
+    <numFmt numFmtId="167" formatCode="0.0\ [$l ]"/>
+    <numFmt numFmtId="168" formatCode="#,##0.00\ [$€-407];[RED]\-#,##0.00\ [$€-407]"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -334,36 +353,50 @@
       <sz val="16"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <i val="true"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -390,8 +423,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFACB20C"/>
+        <bgColor rgb="FF808000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFCC00"/>
       </patternFill>
     </fill>
     <fill>
@@ -412,13 +451,93 @@
         <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000080"/>
+        <bgColor rgb="FF000080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF4D4D4D"/>
+        <bgColor rgb="FF666699"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFD7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFCCCCFF"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="19">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -516,64 +635,106 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -581,23 +742,23 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -605,7 +766,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="7" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -613,72 +774,116 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="12" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="13" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="13" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -751,7 +956,7 @@
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FFCCCCCC"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
@@ -763,7 +968,7 @@
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF7FFF00"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF800000"/>
@@ -779,7 +984,7 @@
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF7FFF00"/>
+      <rgbColor rgb="FFACB20C"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
@@ -792,7 +997,7 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF4D4D4D"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -805,13 +1010,13 @@
       <xdr:col>9</xdr:col>
       <xdr:colOff>47520</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:rowOff>123120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>668160</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>12600</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>110520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -824,8 +1029,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7696800" y="373680"/>
-          <a:ext cx="6305760" cy="6616440"/>
+          <a:off x="7702920" y="373320"/>
+          <a:ext cx="6310440" cy="6616800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -845,9 +1050,9 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>366840</xdr:colOff>
+      <xdr:colOff>366480</xdr:colOff>
       <xdr:row>39</xdr:row>
-      <xdr:rowOff>107280</xdr:rowOff>
+      <xdr:rowOff>106920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
@@ -866,8 +1071,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7357680" y="6702480"/>
-          <a:ext cx="3221640" cy="4203360"/>
+          <a:off x="7363080" y="6702120"/>
+          <a:ext cx="3224520" cy="4203720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -890,7 +1095,7 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>643680</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>147240</xdr:rowOff>
+      <xdr:rowOff>147960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -903,8 +1108,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4576680" y="289440"/>
-          <a:ext cx="6306480" cy="6615360"/>
+          <a:off x="4579920" y="289440"/>
+          <a:ext cx="6311520" cy="6616080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -944,20 +1149,20 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.3"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="5" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="5" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1077,7 +1282,7 @@
         <v>19</v>
       </c>
       <c r="C8" s="7" t="n">
-        <v>25</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1088,591 +1293,585 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="5" t="s">
+    <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="9" t="n">
+        <f aca="false">(L*Br*Ho)/1000-( (4-PI()) *(L*Rb + Br*Rt  )/200)</f>
+        <v>42.5106186954104</v>
+      </c>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="6" t="n">
+      <c r="C11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="6" t="n">
         <f aca="false">PI()/4*D5</f>
         <v>8.63937979737193</v>
       </c>
-      <c r="E10" s="6" t="n">
+      <c r="E11" s="6" t="n">
         <f aca="false">PI()/4*E5</f>
         <v>3.92699081698724</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="10" t="s">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="C13" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="10" t="s">
+      <c r="D13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="H13" s="12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
+      <c r="I13" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="8" t="n">
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="15" t="n">
         <f aca="false">2+ Hs</f>
         <v>22</v>
       </c>
-      <c r="C13" s="8" t="n">
+      <c r="C14" s="16" t="n">
         <f aca="false">2+L+2*Ho -2*Hs-Rt*(4-PI())</f>
-        <v>52.5575191894877</v>
-      </c>
-      <c r="D13" s="8" t="n">
+        <v>62.5575191894877</v>
+      </c>
+      <c r="D14" s="17" t="n">
         <f aca="false">2+L</f>
         <v>52</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="G13" s="8" t="n">
+      <c r="F14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="15" t="n">
         <f aca="false">2+ Hs</f>
         <v>22</v>
       </c>
-      <c r="H13" s="8" t="n">
+      <c r="H14" s="16" t="n">
         <f aca="false">2+L+2*(Ho-Hs)</f>
-        <v>62</v>
-      </c>
-      <c r="I13" s="8" t="n">
+        <v>72</v>
+      </c>
+      <c r="I14" s="17" t="n">
         <f aca="false">2+L</f>
         <v>52</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="8" t="n">
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="18" t="n">
         <f aca="false">2+Br</f>
         <v>32</v>
       </c>
-      <c r="C14" s="8" t="n">
+      <c r="C15" s="19" t="n">
         <f aca="false">2+Br</f>
         <v>32</v>
       </c>
-      <c r="D14" s="8" t="n">
+      <c r="D15" s="20" t="n">
         <f aca="false">2+2*(Ho)+Br-Rb*(4-PI())</f>
-        <v>77.707963267949</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="8" t="n">
+        <v>87.707963267949</v>
+      </c>
+      <c r="F15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" s="18" t="n">
         <f aca="false">2+Br</f>
         <v>32</v>
       </c>
-      <c r="H14" s="8" t="n">
+      <c r="H15" s="19" t="n">
         <f aca="false">2+Br</f>
         <v>32</v>
       </c>
-      <c r="I14" s="8" t="n">
+      <c r="I15" s="20" t="n">
         <f aca="false">2+2*(Ho)+Br</f>
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="8" t="n">
-        <f aca="false">SQRT(B13*B13+B14*B14)</f>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="21" t="n">
+        <f aca="false">SQRT(B14*B14+B15*B15)</f>
         <v>38.8329756778952</v>
       </c>
-      <c r="C15" s="8" t="n">
-        <f aca="false">SQRT(C13*C13+C14*C14)</f>
-        <v>61.5328597040099</v>
-      </c>
-      <c r="D15" s="8" t="n">
-        <f aca="false">SQRT(D13*D13+D14*D14)</f>
-        <v>93.5014842409087</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="8" t="n">
-        <f aca="false">SQRT(G13*G13+G14*G14)</f>
+      <c r="C16" s="22" t="n">
+        <f aca="false">SQRT(C14*C14+C15*C15)</f>
+        <v>70.26694249178</v>
+      </c>
+      <c r="D16" s="23" t="n">
+        <f aca="false">SQRT(D14*D14+D15*D15)</f>
+        <v>101.964144779486</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" s="21" t="n">
+        <f aca="false">SQRT(G14*G14+G15*G15)</f>
         <v>38.8329756778952</v>
       </c>
-      <c r="H15" s="8" t="n">
-        <f aca="false">SQRT(H13*H13+H14*H14)</f>
-        <v>69.7710541700496</v>
-      </c>
-      <c r="I15" s="8" t="n">
-        <f aca="false">SQRT(I13*I13+I14*I14)</f>
-        <v>97.0978887515068</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G16" s="12"/>
+      <c r="H16" s="22" t="n">
+        <f aca="false">SQRT(H14*H14+H15*H15)</f>
+        <v>78.7908624143688</v>
+      </c>
+      <c r="I16" s="23" t="n">
+        <f aca="false">SQRT(I14*I14+I15*I15)</f>
+        <v>105.678758508983</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G17" s="12"/>
+      <c r="G17" s="14"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18" s="10" t="s">
+      <c r="G18" s="14"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="C19" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="D19" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I18" s="13" t="s">
+      <c r="E19" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="24" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C19" s="15" t="n">
+      <c r="I19" s="24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="D19" s="15" t="n">
+      <c r="D20" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G19" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" s="16" t="n">
+      <c r="E20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="I19" s="16" t="n">
+      <c r="I20" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="J19" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="14"/>
-      <c r="C20" s="15" t="n">
+      <c r="J20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="25"/>
+      <c r="C21" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D20" s="15" t="n">
+      <c r="D21" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="G20" s="14"/>
-      <c r="H20" s="16" t="n">
+      <c r="G21" s="25"/>
+      <c r="H21" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="I20" s="16" t="n">
+      <c r="I21" s="27" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="14"/>
-      <c r="C21" s="17" t="n">
-        <f aca="false">C20+E5</f>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="25"/>
+      <c r="C22" s="28" t="n">
+        <f aca="false">C21+E5</f>
         <v>6</v>
       </c>
-      <c r="D21" s="17" t="n">
-        <f aca="false">D20+D5</f>
+      <c r="D22" s="28" t="n">
+        <f aca="false">D21+D5</f>
         <v>12</v>
       </c>
-      <c r="G21" s="14"/>
-      <c r="H21" s="16" t="n">
-        <f aca="false">H20+(Ho -Hs)</f>
-        <v>6</v>
-      </c>
-      <c r="I21" s="16" t="n">
-        <f aca="false">I20+(Ho)</f>
+      <c r="G22" s="25"/>
+      <c r="H22" s="27" t="n">
+        <f aca="false">H21+(Ho -Hs)</f>
+        <v>11</v>
+      </c>
+      <c r="I22" s="27" t="n">
+        <f aca="false">I21+(Ho)</f>
+        <v>31</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="25"/>
+      <c r="C23" s="28" t="n">
+        <f aca="false">C24-$D$11</f>
+        <v>20</v>
+      </c>
+      <c r="D23" s="28" t="n">
+        <f aca="false">D24-$E$11</f>
         <v>26</v>
       </c>
-      <c r="J21" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="14"/>
-      <c r="C22" s="17" t="n">
-        <f aca="false">C23-$D$10</f>
-        <v>15</v>
-      </c>
-      <c r="D22" s="17" t="n">
-        <f aca="false">D23-$E$10</f>
-        <v>21</v>
-      </c>
-      <c r="G22" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="18" t="n">
-        <f aca="false">H21+L/2</f>
-        <v>31</v>
-      </c>
-      <c r="I22" s="18" t="n">
-        <f aca="false">I21+Br / 2</f>
+      <c r="G23" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="29" t="n">
+        <f aca="false">H22+L/2</f>
+        <v>36</v>
+      </c>
+      <c r="I23" s="29" t="n">
+        <f aca="false">I22+Br / 2</f>
+        <v>46</v>
+      </c>
+      <c r="J23" s="30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C24" s="26" t="n">
+        <f aca="false">C21+Ho-Rt*(1-PI()/4)</f>
+        <v>28.6393797973719</v>
+      </c>
+      <c r="D24" s="26" t="n">
+        <f aca="false">D21+Ho-Rb*(1-PI()/4)</f>
+        <v>29.9269908169872</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="H24" s="27" t="n">
+        <f aca="false">H22+L</f>
+        <v>61</v>
+      </c>
+      <c r="I24" s="27" t="n">
+        <f aca="false">I22+Br</f>
+        <v>61</v>
+      </c>
+      <c r="J24" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="J22" s="19" t="s">
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="25"/>
+      <c r="C25" s="28" t="n">
+        <f aca="false">C24+$D$11</f>
+        <v>37.2787595947439</v>
+      </c>
+      <c r="D25" s="28" t="n">
+        <f aca="false">D24+$E$11</f>
+        <v>33.8539816339745</v>
+      </c>
+      <c r="G25" s="25"/>
+      <c r="H25" s="27" t="n">
+        <f aca="false">H24+(Ho -Hs)</f>
+        <v>71</v>
+      </c>
+      <c r="I25" s="27" t="n">
+        <f aca="false">I24+(Ho)</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="25" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="15" t="n">
-        <f aca="false">C20+Ho-Rt*(1-PI()/4)</f>
-        <v>23.6393797973719</v>
-      </c>
-      <c r="D23" s="15" t="n">
-        <f aca="false">D20+Ho-Rb*(1-PI()/4)</f>
-        <v>24.9269908169872</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="H23" s="16" t="n">
-        <f aca="false">H21+L</f>
-        <v>56</v>
-      </c>
-      <c r="I23" s="16" t="n">
-        <f aca="false">I21+Br</f>
-        <v>56</v>
-      </c>
-      <c r="J23" s="19" t="s">
+      <c r="C26" s="26" t="n">
+        <f aca="false">C24+L/2-Rt*(1-PI()/4)</f>
+        <v>51.2787595947439</v>
+      </c>
+      <c r="D26" s="26" t="n">
+        <f aca="false">D24+Br/2-Rb*(1-PI()/4)</f>
+        <v>43.8539816339745</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="H26" s="27" t="n">
+        <f aca="false">H25+1</f>
+        <v>72</v>
+      </c>
+      <c r="I26" s="27" t="n">
+        <f aca="false">I25+1</f>
+        <v>92</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="25"/>
+      <c r="C27" s="28" t="n">
+        <f aca="false">C28-$D$11</f>
+        <v>65.2787595947439</v>
+      </c>
+      <c r="D27" s="28" t="n">
+        <f aca="false">D28-$E$11</f>
+        <v>53.8539816339745</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="25" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="14"/>
-      <c r="C24" s="17" t="n">
-        <f aca="false">C23+$D$10</f>
-        <v>32.2787595947439</v>
-      </c>
-      <c r="D24" s="17" t="n">
-        <f aca="false">D23+$E$10</f>
-        <v>28.8539816339745</v>
-      </c>
-      <c r="G24" s="14"/>
-      <c r="H24" s="16" t="n">
-        <f aca="false">H23+(Ho -Hs)</f>
-        <v>61</v>
-      </c>
-      <c r="I24" s="16" t="n">
-        <f aca="false">I23+(Ho)</f>
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="15" t="n">
-        <f aca="false">C23+L/2-Rt*(1-PI()/4)</f>
-        <v>46.2787595947439</v>
-      </c>
-      <c r="D25" s="15" t="n">
-        <f aca="false">D23+Br/2-Rb*(1-PI()/4)</f>
-        <v>38.8539816339745</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="G25" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="H25" s="16" t="n">
-        <f aca="false">H24+1</f>
-        <v>62</v>
-      </c>
-      <c r="I25" s="16" t="n">
-        <f aca="false">I24+1</f>
-        <v>82</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="14"/>
-      <c r="C26" s="17" t="n">
-        <f aca="false">C27-$D$10</f>
-        <v>60.2787595947439</v>
-      </c>
-      <c r="D26" s="17" t="n">
-        <f aca="false">D27-$E$10</f>
-        <v>48.8539816339745</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C27" s="15" t="n">
-        <f aca="false">C25+L/2-Rt*(1-PI()/4)</f>
-        <v>68.9181393921158</v>
-      </c>
-      <c r="D27" s="15" t="n">
-        <f aca="false">D25+Br/2-Rb*(1-PI()/4)</f>
-        <v>52.7809724509617</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="14"/>
-      <c r="C28" s="17" t="n">
-        <f aca="false">C27+$D$10</f>
-        <v>77.5575191894877</v>
-      </c>
-      <c r="D28" s="17" t="n">
-        <f aca="false">D27+$E$10</f>
-        <v>56.707963267949</v>
+      <c r="C28" s="26" t="n">
+        <f aca="false">C26+L/2-Rt*(1-PI()/4)</f>
+        <v>73.9181393921158</v>
+      </c>
+      <c r="D28" s="26" t="n">
+        <f aca="false">D26+Br/2-Rb*(1-PI()/4)</f>
+        <v>57.7809724509617</v>
+      </c>
+      <c r="E28" s="30" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="14"/>
-      <c r="C29" s="17" t="n">
-        <f aca="false">C30-$E$5</f>
-        <v>86.5575191894877</v>
-      </c>
-      <c r="D29" s="17" t="n">
-        <f aca="false">D30-$D$5</f>
-        <v>65.707963267949</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>44</v>
+      <c r="B29" s="25"/>
+      <c r="C29" s="28" t="n">
+        <f aca="false">C28+$D$11</f>
+        <v>82.5575191894877</v>
+      </c>
+      <c r="D29" s="28" t="n">
+        <f aca="false">D28+$E$11</f>
+        <v>61.707963267949</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="14"/>
-      <c r="C30" s="15" t="n">
-        <f aca="false">C27+Ho-Rt*(1-PI()/4)</f>
-        <v>91.5575191894877</v>
-      </c>
-      <c r="D30" s="15" t="n">
-        <f aca="false">D27+Ho-Rb*(1-PI()/4)</f>
-        <v>76.707963267949</v>
-      </c>
-      <c r="E30" s="19"/>
+      <c r="B30" s="25"/>
+      <c r="C30" s="28" t="n">
+        <f aca="false">C31-$E$5</f>
+        <v>96.5575191894877</v>
+      </c>
+      <c r="D30" s="28" t="n">
+        <f aca="false">D31-$D$5</f>
+        <v>75.707963267949</v>
+      </c>
       <c r="F30" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="15" t="n">
-        <f aca="false">C30+1</f>
-        <v>92.5575191894877</v>
-      </c>
-      <c r="D31" s="15" t="n">
-        <f aca="false">D30+1</f>
-        <v>77.707963267949</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>42</v>
-      </c>
-      <c r="G31" s="8"/>
+      <c r="B31" s="25"/>
+      <c r="C31" s="26" t="n">
+        <f aca="false">C28+Ho-Rt*(1-PI()/4)</f>
+        <v>101.557519189488</v>
+      </c>
+      <c r="D31" s="26" t="n">
+        <f aca="false">D28+Ho-Rb*(1-PI()/4)</f>
+        <v>86.707963267949</v>
+      </c>
+      <c r="E31" s="30"/>
+      <c r="F31" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="14"/>
+      <c r="B32" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C32" s="26" t="n">
+        <f aca="false">C31+1</f>
+        <v>102.557519189488</v>
+      </c>
+      <c r="D32" s="26" t="n">
+        <f aca="false">D31+1</f>
+        <v>87.707963267949</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>43</v>
+      </c>
       <c r="G32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="14"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="14"/>
-      <c r="C34" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D34" s="10" t="s">
+      <c r="B33" s="25"/>
+      <c r="G33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="25"/>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="25"/>
+      <c r="C35" s="12" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="17" t="n">
+      <c r="D35" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="D35" s="17" t="n">
+      <c r="D36" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="14"/>
-      <c r="C36" s="17" t="n">
+      <c r="E36" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="25"/>
+      <c r="C37" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="D36" s="17" t="n">
+      <c r="D37" s="28" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="14"/>
-      <c r="C37" s="17" t="n">
-        <f aca="false">C36+$E$5</f>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="25"/>
+      <c r="C38" s="28" t="n">
+        <f aca="false">C37+$E$5</f>
         <v>6</v>
       </c>
-      <c r="D37" s="17" t="n">
-        <f aca="false">D36+$D$5</f>
+      <c r="D38" s="28" t="n">
+        <f aca="false">D37+$D$5</f>
         <v>12</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="14" t="n">
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B39" s="25" t="n">
         <v>9.3</v>
       </c>
-      <c r="C38" s="17" t="n">
-        <f aca="false">C36+Br/2</f>
+      <c r="C39" s="28" t="n">
+        <f aca="false">C37+Br/2</f>
         <v>16</v>
       </c>
-      <c r="D38" s="17" t="n">
-        <f aca="false">D36+L/2</f>
+      <c r="D39" s="28" t="n">
+        <f aca="false">D37+L/2</f>
         <v>26</v>
       </c>
-      <c r="E38" s="1" t="n">
+      <c r="E39" s="1" t="n">
         <v>12.6</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="14"/>
-      <c r="C39" s="17" t="n">
-        <f aca="false">C40-$E$5</f>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B40" s="25"/>
+      <c r="C40" s="28" t="n">
+        <f aca="false">C41-$E$5</f>
         <v>26</v>
       </c>
-      <c r="D39" s="17" t="n">
-        <f aca="false">D40-$D$5</f>
+      <c r="D40" s="28" t="n">
+        <f aca="false">D41-$D$5</f>
         <v>40</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="14"/>
-      <c r="C40" s="17" t="n">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="25"/>
+      <c r="C41" s="28" t="n">
         <f aca="false">Br + 1</f>
         <v>31</v>
       </c>
-      <c r="D40" s="17" t="n">
+      <c r="D41" s="28" t="n">
         <f aca="false">L + 1</f>
         <v>51</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C41" s="17" t="n">
-        <f aca="false">C40+1</f>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B42" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C42" s="28" t="n">
+        <f aca="false">C41+1</f>
         <v>32</v>
       </c>
-      <c r="D41" s="17" t="n">
-        <f aca="false">D40+1</f>
+      <c r="D42" s="28" t="n">
+        <f aca="false">D41+1</f>
         <v>52</v>
       </c>
-      <c r="E41" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
+      <c r="E42" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H42" s="19"/>
+      <c r="I42" s="19"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I57" s="8" t="n">
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H48" s="19"/>
+      <c r="I48" s="19"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I58" s="19" t="n">
         <f aca="false">2+L+2*Ho -Rt*(4-PI())</f>
-        <v>92.5575191894877</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="G60" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="H60" s="1" t="n">
-        <f aca="false">$G$72 - G60</f>
-        <v>103.845130209103</v>
-      </c>
-      <c r="I60" s="1" t="n">
-        <f aca="false">H60+G60</f>
-        <v>103.845130209103</v>
-      </c>
-      <c r="J60" s="1" t="n">
-        <f aca="false">(60.6-18)/2</f>
-        <v>21.3</v>
+        <v>102.557519189488</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F61" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G61" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H61" s="1" t="n">
-        <f aca="false">$G$72 - G61</f>
-        <v>102.845130209103</v>
+        <f aca="false">$G$73 - G61</f>
+        <v>103.845130209103</v>
       </c>
       <c r="I61" s="1" t="n">
         <f aca="false">H61+G61</f>
         <v>103.845130209103</v>
       </c>
+      <c r="J61" s="1" t="n">
+        <f aca="false">(60.6-18)/2</f>
+        <v>21.3</v>
+      </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F62" s="1" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G62" s="1" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="H62" s="1" t="n">
-        <f aca="false">$G$72 - G62</f>
-        <v>97.845130209103</v>
+        <f aca="false">$G$73 - G62</f>
+        <v>102.845130209103</v>
       </c>
       <c r="I62" s="1" t="n">
         <f aca="false">H62+G62</f>
@@ -1681,14 +1880,14 @@
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F63" s="1" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="G63" s="1" t="n">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="H63" s="1" t="n">
-        <f aca="false">$G$72 - G63</f>
-        <v>83.845130209103</v>
+        <f aca="false">$G$73 - G63</f>
+        <v>97.845130209103</v>
       </c>
       <c r="I63" s="1" t="n">
         <f aca="false">H63+G63</f>
@@ -1697,14 +1896,14 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F64" s="1" t="n">
-        <v>28.6393797973719</v>
+        <v>20</v>
       </c>
       <c r="G64" s="1" t="n">
-        <v>28.6393797973719</v>
+        <v>20</v>
       </c>
       <c r="H64" s="1" t="n">
-        <f aca="false">$G$72 - G64</f>
-        <v>75.2057504117311</v>
+        <f aca="false">$G$73 - G64</f>
+        <v>83.845130209103</v>
       </c>
       <c r="I64" s="1" t="n">
         <f aca="false">H64+G64</f>
@@ -1713,14 +1912,14 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F65" s="1" t="n">
-        <v>37.2787595947439</v>
+        <v>28.6393797973719</v>
       </c>
       <c r="G65" s="1" t="n">
-        <v>37.2787595947439</v>
+        <v>28.6393797973719</v>
       </c>
       <c r="H65" s="1" t="n">
-        <f aca="false">$G$72 - G65</f>
-        <v>66.5663706143591</v>
+        <f aca="false">$G$73 - G65</f>
+        <v>75.2057504117311</v>
       </c>
       <c r="I65" s="1" t="n">
         <f aca="false">H65+G65</f>
@@ -1729,14 +1928,14 @@
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F66" s="1" t="n">
-        <v>51.2787595947439</v>
+        <v>37.2787595947439</v>
       </c>
       <c r="G66" s="1" t="n">
-        <v>51.2787595947439</v>
+        <v>37.2787595947439</v>
       </c>
       <c r="H66" s="1" t="n">
-        <f aca="false">$G$72 - G66</f>
-        <v>52.5663706143591</v>
+        <f aca="false">$G$73 - G66</f>
+        <v>66.5663706143591</v>
       </c>
       <c r="I66" s="1" t="n">
         <f aca="false">H66+G66</f>
@@ -1745,14 +1944,14 @@
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F67" s="1" t="n">
-        <v>65.2787595947439</v>
+        <v>51.2787595947439</v>
       </c>
       <c r="G67" s="1" t="n">
-        <v>65.2787595947439</v>
+        <v>51.2787595947439</v>
       </c>
       <c r="H67" s="1" t="n">
-        <f aca="false">$G$72 - G67</f>
-        <v>38.5663706143591</v>
+        <f aca="false">$G$73 - G67</f>
+        <v>52.5663706143591</v>
       </c>
       <c r="I67" s="1" t="n">
         <f aca="false">H67+G67</f>
@@ -1761,14 +1960,14 @@
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F68" s="1" t="n">
-        <v>73.9181393921158</v>
+        <v>65.2787595947439</v>
       </c>
       <c r="G68" s="1" t="n">
-        <v>73.9181393921158</v>
+        <v>65.2787595947439</v>
       </c>
       <c r="H68" s="1" t="n">
-        <f aca="false">$G$72 - G68</f>
-        <v>29.9269908169872</v>
+        <f aca="false">$G$73 - G68</f>
+        <v>38.5663706143591</v>
       </c>
       <c r="I68" s="1" t="n">
         <f aca="false">H68+G68</f>
@@ -1777,14 +1976,14 @@
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F69" s="1" t="n">
-        <v>82.5575191894877</v>
+        <v>73.9181393921158</v>
       </c>
       <c r="G69" s="1" t="n">
-        <v>82.5575191894877</v>
+        <v>73.9181393921158</v>
       </c>
       <c r="H69" s="1" t="n">
-        <f aca="false">$G$72 - G69</f>
-        <v>21.2876110196153</v>
+        <f aca="false">$G$73 - G69</f>
+        <v>29.9269908169872</v>
       </c>
       <c r="I69" s="1" t="n">
         <f aca="false">H69+G69</f>
@@ -1793,14 +1992,14 @@
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F70" s="1" t="n">
-        <v>97.845130209103</v>
+        <v>82.5575191894877</v>
       </c>
       <c r="G70" s="1" t="n">
-        <v>97.845130209103</v>
+        <v>82.5575191894877</v>
       </c>
       <c r="H70" s="1" t="n">
-        <f aca="false">$G$72 - G70</f>
-        <v>6</v>
+        <f aca="false">$G$73 - G70</f>
+        <v>21.2876110196153</v>
       </c>
       <c r="I70" s="1" t="n">
         <f aca="false">H70+G70</f>
@@ -1809,14 +2008,14 @@
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F71" s="1" t="n">
-        <v>102.845130209103</v>
+        <v>97.845130209103</v>
       </c>
       <c r="G71" s="1" t="n">
-        <v>102.845130209103</v>
+        <v>97.845130209103</v>
       </c>
       <c r="H71" s="1" t="n">
-        <f aca="false">$G$72 - G71</f>
-        <v>1</v>
+        <f aca="false">$G$73 - G71</f>
+        <v>6</v>
       </c>
       <c r="I71" s="1" t="n">
         <f aca="false">H71+G71</f>
@@ -1825,17 +2024,33 @@
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F72" s="1" t="n">
-        <v>103.845130209103</v>
+        <v>102.845130209103</v>
       </c>
       <c r="G72" s="1" t="n">
-        <v>103.845130209103</v>
+        <v>102.845130209103</v>
       </c>
       <c r="H72" s="1" t="n">
-        <f aca="false">$G$72 - G72</f>
-        <v>0</v>
+        <f aca="false">$G$73 - G72</f>
+        <v>1</v>
       </c>
       <c r="I72" s="1" t="n">
         <f aca="false">H72+G72</f>
+        <v>103.845130209103</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F73" s="1" t="n">
+        <v>103.845130209103</v>
+      </c>
+      <c r="G73" s="1" t="n">
+        <v>103.845130209103</v>
+      </c>
+      <c r="H73" s="1" t="n">
+        <f aca="false">$G$73 - G73</f>
+        <v>0</v>
+      </c>
+      <c r="I73" s="1" t="n">
+        <f aca="false">H73+G73</f>
         <v>103.845130209103</v>
       </c>
     </row>
@@ -1851,11 +2066,13 @@
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  <pageMargins left="0.7875" right="0.7875" top="0.886111111111111" bottom="0.886111111111111" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="true" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CSeite &amp;P</oddFooter>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -1864,22 +2081,22 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+    <pageSetUpPr fitToPage="true"/>
   </sheetPr>
   <dimension ref="B1:S67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L57" activeCellId="0" sqref="L57"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.28"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.26"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="3" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.27"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="9" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1898,17 +2115,17 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="20" t="s">
+      <c r="E4" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="31" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1916,15 +2133,15 @@
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="25" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="21" t="n">
+      <c r="E5" s="32" t="n">
         <f aca="false">Rt</f>
         <v>11</v>
       </c>
-      <c r="F5" s="21" t="n">
+      <c r="F5" s="32" t="n">
         <f aca="false">Rb</f>
         <v>5</v>
       </c>
@@ -1937,11 +2154,11 @@
       <c r="I5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="22" t="n">
+      <c r="J5" s="33" t="n">
         <f aca="false">$E$5*(2-PI()/2)</f>
         <v>4.72124040525614</v>
       </c>
-      <c r="K5" s="22" t="n">
+      <c r="K5" s="33" t="n">
         <f aca="false">$F$5*(2-PI()/2)</f>
         <v>2.14601836602552</v>
       </c>
@@ -1953,10 +2170,10 @@
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="21" t="n">
+      <c r="D6" s="32" t="n">
         <f aca="false">L</f>
         <v>50</v>
       </c>
@@ -1966,11 +2183,11 @@
         <v>14</v>
       </c>
       <c r="I6" s="5"/>
-      <c r="J6" s="22" t="n">
+      <c r="J6" s="33" t="n">
         <f aca="false">J5*2</f>
         <v>9.44248081051228</v>
       </c>
-      <c r="K6" s="22" t="n">
+      <c r="K6" s="33" t="n">
         <f aca="false">K5*2</f>
         <v>4.29203673205103</v>
       </c>
@@ -1982,25 +2199,25 @@
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="21" t="n">
+      <c r="D7" s="32" t="n">
         <f aca="false">Br</f>
         <v>30</v>
       </c>
-      <c r="E7" s="23" t="s">
-        <v>49</v>
+      <c r="E7" s="34" t="s">
+        <v>50</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="J7" s="22" t="n">
+      <c r="J7" s="33" t="n">
         <f aca="false">J6*2</f>
         <v>18.8849616210246</v>
       </c>
-      <c r="K7" s="22" t="n">
+      <c r="K7" s="33" t="n">
         <f aca="false">K6*2</f>
         <v>8.58407346410207</v>
       </c>
@@ -2008,47 +2225,47 @@
         <v>20</v>
       </c>
       <c r="Q7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="R7" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="S7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="21" t="n">
-        <f aca="false">Ho</f>
-        <v>25</v>
-      </c>
-      <c r="E8" s="23" t="s">
+      <c r="C8" s="31" t="s">
         <v>54</v>
       </c>
+      <c r="D8" s="32" t="n">
+        <f aca="false"> Ho</f>
+        <v>30</v>
+      </c>
+      <c r="E8" s="34" t="s">
+        <v>55</v>
+      </c>
       <c r="H8" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J8" s="22" t="n">
+        <v>23</v>
+      </c>
+      <c r="J8" s="33" t="n">
         <f aca="false">PI()/4*E5</f>
         <v>8.63937979737193</v>
       </c>
-      <c r="K8" s="22" t="n">
+      <c r="K8" s="33" t="n">
         <f aca="false">PI()/4*F5</f>
         <v>3.92699081698724</v>
       </c>
       <c r="Q8" s="8" t="n">
         <v>40</v>
       </c>
-      <c r="R8" s="3" t="n">
+      <c r="R8" s="35" t="n">
         <f aca="false">PI()/4*Q8*Q8</f>
         <v>1256.63706143592</v>
       </c>
@@ -2060,24 +2277,24 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="5"/>
       <c r="C9" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D9" s="6" t="n">
         <f aca="false">D8*D7</f>
-        <v>750</v>
+        <v>900</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="9"/>
-      <c r="C10" s="24" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="25" t="s">
+      <c r="B10" s="11"/>
+      <c r="C10" s="36" t="s">
         <v>25</v>
       </c>
-      <c r="E10" s="26" t="s">
-        <v>56</v>
+      <c r="D10" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="38" t="s">
+        <v>57</v>
       </c>
       <c r="R10" s="1" t="n">
         <f aca="false">SQRT(PI()/4)</f>
@@ -2086,54 +2303,54 @@
       <c r="S10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="27" t="n">
+      <c r="B11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="39" t="n">
         <f aca="false">2+L+Ho -Rt*(4-PI())/2</f>
-        <v>72.2787595947439</v>
-      </c>
-      <c r="D11" s="28" t="n">
+        <v>77.2787595947439</v>
+      </c>
+      <c r="D11" s="40" t="n">
         <f aca="false">2+L</f>
         <v>52</v>
       </c>
-      <c r="E11" s="29" t="n">
+      <c r="E11" s="41" t="n">
         <f aca="false">G18+2</f>
-        <v>29.1460183660255</v>
+        <v>34.1460183660255</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="C12" s="27" t="n">
+      <c r="B12" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="39" t="n">
         <f aca="false">2+Br</f>
         <v>32</v>
       </c>
-      <c r="D12" s="28" t="n">
+      <c r="D12" s="40" t="n">
         <f aca="false">2+2*(Ho)+Br-Rb*(4-PI())</f>
-        <v>77.707963267949</v>
-      </c>
-      <c r="E12" s="29" t="n">
+        <v>87.707963267949</v>
+      </c>
+      <c r="E12" s="42" t="n">
         <f aca="false">2+Br</f>
         <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C13" s="30" t="n">
+      <c r="B13" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="43" t="n">
         <f aca="false">SQRT(C11*C11+C12*C12)</f>
-        <v>79.0456772287693</v>
-      </c>
-      <c r="D13" s="31" t="n">
+        <v>83.6421346242563</v>
+      </c>
+      <c r="D13" s="44" t="n">
         <f aca="false">SQRT(D11*D11+D12*D12)</f>
-        <v>93.5014842409087</v>
-      </c>
-      <c r="E13" s="32" t="n">
+        <v>101.964144779486</v>
+      </c>
+      <c r="E13" s="45" t="n">
         <f aca="false">SQRT(E11*E11+E12*E12)</f>
-        <v>43.2838351650209</v>
+        <v>46.7969076996862</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2143,255 +2360,255 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C16" s="10" t="s">
+      <c r="B16" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="C16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="D16" s="12" t="s">
         <v>32</v>
       </c>
+      <c r="E16" s="12" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15" t="n">
+      <c r="B17" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G17" s="8" t="n">
         <f aca="false">D29-2+D7</f>
-        <v>105.707963267949</v>
+        <v>115.707963267949</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="14"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15" t="n">
+      <c r="B18" s="25"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="33" t="n">
+        <v>59</v>
+      </c>
+      <c r="G18" s="46" t="n">
         <f aca="false">(G17+K7-2*D7)/2</f>
-        <v>27.1460183660255</v>
+        <v>32.1460183660255</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="14"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17" t="n">
+      <c r="B19" s="25"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28" t="n">
         <f aca="false">D18+E5</f>
         <v>12</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="14"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17" t="n">
+      <c r="B20" s="25"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28" t="n">
         <f aca="false">D21-$K$8</f>
-        <v>21</v>
-      </c>
-      <c r="G20" s="34"/>
+        <v>26</v>
+      </c>
+      <c r="G20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="C21" s="15" t="n">
+      <c r="B21" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="15" t="n">
+      <c r="D21" s="26" t="n">
         <f aca="false">D18+Ho-Rb*(1-PI()/4)</f>
-        <v>24.9269908169872</v>
+        <v>29.9269908169872</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="34"/>
+        <v>39</v>
+      </c>
+      <c r="G21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="14"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="17" t="n">
+      <c r="B22" s="25"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28" t="n">
         <f aca="false">D21+$K$8</f>
-        <v>28.8539816339745</v>
+        <v>33.8539816339745</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="15" t="n">
+      <c r="B23" s="25" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="26" t="n">
         <f aca="false">C21+L/2</f>
         <v>26</v>
       </c>
-      <c r="D23" s="15" t="n">
+      <c r="D23" s="26" t="n">
         <f aca="false">D21+Br/2-Rb*(1-PI()/4)</f>
-        <v>38.8539816339745</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>41</v>
+        <v>43.8539816339745</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="14"/>
-      <c r="C24" s="17" t="n">
+      <c r="B24" s="25"/>
+      <c r="C24" s="28" t="n">
         <f aca="false">C25-$J$8</f>
         <v>40</v>
       </c>
-      <c r="D24" s="17" t="n">
+      <c r="D24" s="28" t="n">
         <f aca="false">D25-$K$8</f>
-        <v>48.8539816339745</v>
+        <v>53.8539816339745</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="C25" s="15" t="n">
+      <c r="B25" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="C25" s="26" t="n">
         <f aca="false">C23+L/2-Rt*(1-PI()/4)</f>
         <v>48.6393797973719</v>
       </c>
-      <c r="D25" s="15" t="n">
+      <c r="D25" s="26" t="n">
         <f aca="false">D23+Br/2-Rb*(1-PI()/4)</f>
-        <v>52.7809724509617</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>43</v>
+        <v>57.7809724509617</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="14"/>
-      <c r="C26" s="17" t="n">
+      <c r="B26" s="25"/>
+      <c r="C26" s="28" t="n">
         <f aca="false">C25+$J$8</f>
         <v>57.2787595947439</v>
       </c>
-      <c r="D26" s="17" t="n">
+      <c r="D26" s="28" t="n">
         <f aca="false">D25+$K$8</f>
-        <v>56.707963267949</v>
+        <v>61.707963267949</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14"/>
-      <c r="C27" s="17" t="n">
+      <c r="B27" s="25"/>
+      <c r="C27" s="28" t="n">
         <f aca="false">C28-$F$5</f>
-        <v>66.2787595947439</v>
-      </c>
-      <c r="D27" s="17" t="n">
+        <v>71.2787595947439</v>
+      </c>
+      <c r="D27" s="28" t="n">
         <f aca="false">D28-$E$5</f>
-        <v>65.707963267949</v>
+        <v>75.707963267949</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="14"/>
-      <c r="C28" s="15" t="n">
+      <c r="B28" s="25"/>
+      <c r="C28" s="26" t="n">
         <f aca="false">C25+Ho-Rt*(1-PI()/4)</f>
-        <v>71.2787595947439</v>
-      </c>
-      <c r="D28" s="15" t="n">
+        <v>76.2787595947439</v>
+      </c>
+      <c r="D28" s="26" t="n">
         <f aca="false">D25+Ho-Rb*(1-PI()/4)</f>
-        <v>76.707963267949</v>
-      </c>
-      <c r="E28" s="19"/>
+        <v>86.707963267949</v>
+      </c>
+      <c r="E28" s="30"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C29" s="15" t="n">
+      <c r="B29" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C29" s="26" t="n">
         <f aca="false">C28+1</f>
-        <v>72.2787595947439</v>
-      </c>
-      <c r="D29" s="15" t="n">
+        <v>77.2787595947439</v>
+      </c>
+      <c r="D29" s="26" t="n">
         <f aca="false">D28+1</f>
-        <v>77.707963267949</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>42</v>
+        <v>87.707963267949</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>43</v>
       </c>
       <c r="G29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="14"/>
+      <c r="B30" s="25"/>
       <c r="C30" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="14"/>
+      <c r="B31" s="25"/>
       <c r="E31" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="14"/>
-      <c r="C32" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="10" t="s">
+      <c r="B32" s="25"/>
+      <c r="C32" s="12" t="s">
         <v>47</v>
       </c>
+      <c r="D32" s="12" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C33" s="17" t="n">
+      <c r="B33" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="C33" s="28" t="n">
         <v>0</v>
       </c>
-      <c r="D33" s="17" t="n">
+      <c r="D33" s="28" t="n">
         <v>0</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="14"/>
-      <c r="C34" s="17" t="n">
+      <c r="B34" s="25"/>
+      <c r="C34" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="D34" s="17" t="n">
+      <c r="D34" s="28" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="14"/>
-      <c r="C35" s="17" t="n">
+      <c r="B35" s="25"/>
+      <c r="C35" s="28" t="n">
         <f aca="false">C34+$F$5</f>
         <v>6</v>
       </c>
-      <c r="D35" s="17"/>
+      <c r="D35" s="28"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="14" t="n">
+      <c r="B36" s="25" t="n">
         <v>9.3</v>
       </c>
-      <c r="C36" s="17" t="n">
+      <c r="C36" s="28" t="n">
         <f aca="false">C34+Br/2</f>
         <v>16</v>
       </c>
-      <c r="D36" s="17" t="n">
+      <c r="D36" s="28" t="n">
         <f aca="false">D34+L/2</f>
         <v>26</v>
       </c>
@@ -2400,67 +2617,67 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="14"/>
-      <c r="C37" s="17" t="n">
+      <c r="B37" s="25"/>
+      <c r="C37" s="28" t="n">
         <f aca="false">C38-$F$5</f>
         <v>26</v>
       </c>
-      <c r="D37" s="17" t="n">
+      <c r="D37" s="28" t="n">
         <f aca="false">D38-$E$5</f>
         <v>40</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="14"/>
-      <c r="C38" s="17" t="n">
+      <c r="B38" s="25"/>
+      <c r="C38" s="28" t="n">
         <f aca="false">Br + 1</f>
         <v>31</v>
       </c>
-      <c r="D38" s="17" t="n">
+      <c r="D38" s="28" t="n">
         <f aca="false">L + 1</f>
         <v>51</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C39" s="17" t="n">
+      <c r="B39" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="28" t="n">
         <f aca="false">C38+1</f>
         <v>32</v>
       </c>
-      <c r="D39" s="17" t="n">
+      <c r="D39" s="28" t="n">
         <f aca="false">D38+1</f>
         <v>52</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
+        <v>43</v>
+      </c>
+      <c r="H39" s="19"/>
+      <c r="I39" s="19"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C42" s="2"/>
-      <c r="G42" s="19"/>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
+      <c r="G42" s="30"/>
+      <c r="H42" s="30"/>
+      <c r="I42" s="30"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G43" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="I43" s="19"/>
+        <v>64</v>
+      </c>
+      <c r="I43" s="30"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1" t="s">
@@ -2470,28 +2687,28 @@
         <v>3</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H44" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="I44" s="34"/>
+      <c r="I44" s="47"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G45" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H45" s="8" t="n">
         <f aca="false">$D$47/2-E$46</f>
         <v>10</v>
       </c>
-      <c r="I45" s="34"/>
+      <c r="I45" s="47"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="31" t="s">
         <v>8</v>
       </c>
       <c r="D46" s="3"/>
@@ -2499,74 +2716,74 @@
         <f aca="false">F5</f>
         <v>5</v>
       </c>
-      <c r="G46" s="35" t="s">
-        <v>66</v>
-      </c>
-      <c r="H46" s="36" t="n">
+      <c r="G46" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="H46" s="49" t="n">
         <f aca="false">H45+E$49</f>
         <v>13.9269908169872</v>
       </c>
-      <c r="I46" s="34"/>
+      <c r="I46" s="47"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="D47" s="33" t="n">
+      <c r="C47" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" s="46" t="n">
         <f aca="false">D7</f>
         <v>30</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H47" s="8" t="n">
         <f aca="false">H46+E$49</f>
         <v>17.8539816339745</v>
       </c>
-      <c r="I47" s="19"/>
+      <c r="I47" s="30"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="D48" s="33" t="n">
+      <c r="C48" s="31" t="s">
+        <v>70</v>
+      </c>
+      <c r="D48" s="46" t="n">
         <f aca="false">G18</f>
-        <v>27.1460183660255</v>
-      </c>
-      <c r="G48" s="35" t="s">
-        <v>70</v>
-      </c>
-      <c r="H48" s="36" t="n">
+        <v>32.1460183660255</v>
+      </c>
+      <c r="G48" s="48" t="s">
+        <v>71</v>
+      </c>
+      <c r="H48" s="49" t="n">
         <f aca="false">H47+$D$48/2-E$46</f>
-        <v>26.4269908169872</v>
-      </c>
-      <c r="I48" s="19"/>
+        <v>28.9269908169872</v>
+      </c>
+      <c r="I48" s="30"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E49" s="8" t="n">
         <f aca="false">PI()/4*E46</f>
         <v>3.92699081698724</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H49" s="8" t="n">
         <f aca="false">H48+$D$48/2-E$46</f>
-        <v>35</v>
-      </c>
-      <c r="I49" s="19"/>
+        <v>40</v>
+      </c>
+      <c r="I49" s="30"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="1" t="s">
@@ -2582,14 +2799,14 @@
         <f aca="false">E$46*(2-PI()/2)</f>
         <v>2.14601836602552</v>
       </c>
-      <c r="G50" s="35" t="s">
-        <v>72</v>
-      </c>
-      <c r="H50" s="36" t="n">
+      <c r="G50" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="H50" s="49" t="n">
         <f aca="false">H49+E$49</f>
-        <v>38.9269908169872</v>
-      </c>
-      <c r="I50" s="19"/>
+        <v>43.9269908169872</v>
+      </c>
+      <c r="I50" s="30"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="1" t="s">
@@ -2600,13 +2817,13 @@
         <v>4.29203673205103</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H51" s="8" t="n">
         <f aca="false">H50+E$49</f>
-        <v>42.8539816339745</v>
-      </c>
-      <c r="I51" s="19"/>
+        <v>47.8539816339745</v>
+      </c>
+      <c r="I51" s="30"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="1" t="s">
@@ -2616,154 +2833,154 @@
         <f aca="false">E51*2</f>
         <v>8.58407346410207</v>
       </c>
-      <c r="G52" s="35" t="s">
-        <v>74</v>
-      </c>
-      <c r="H52" s="36" t="n">
+      <c r="G52" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="H52" s="49" t="n">
         <f aca="false">H51+$D$47/2-E$46</f>
-        <v>52.8539816339745</v>
-      </c>
-      <c r="I52" s="19"/>
+        <v>57.8539816339745</v>
+      </c>
+      <c r="I52" s="30"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G53" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H53" s="8" t="n">
         <f aca="false">H52+$D$47/2-E$46</f>
-        <v>62.8539816339745</v>
-      </c>
-      <c r="I53" s="19"/>
+        <v>67.8539816339745</v>
+      </c>
+      <c r="I53" s="30"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G54" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="H54" s="36" t="n">
+      <c r="G54" s="48" t="s">
+        <v>77</v>
+      </c>
+      <c r="H54" s="49" t="n">
         <f aca="false">H53+E$49</f>
-        <v>66.7809724509617</v>
-      </c>
-      <c r="I54" s="19"/>
+        <v>71.7809724509617</v>
+      </c>
+      <c r="I54" s="30"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G55" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H55" s="8" t="n">
         <f aca="false">H54+E$49</f>
-        <v>70.707963267949</v>
-      </c>
-      <c r="I55" s="19"/>
+        <v>75.707963267949</v>
+      </c>
+      <c r="I55" s="30"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G56" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="H56" s="36" t="n">
+      <c r="G56" s="48" t="s">
+        <v>79</v>
+      </c>
+      <c r="H56" s="49" t="n">
         <f aca="false">H55+$D$48/2-E$46</f>
-        <v>79.2809724509617</v>
-      </c>
-      <c r="I56" s="19"/>
+        <v>86.7809724509617</v>
+      </c>
+      <c r="I56" s="30"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G57" s="1" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H57" s="8" t="n">
         <f aca="false">H56+$D$48/2-E$46</f>
-        <v>87.8539816339745</v>
-      </c>
-      <c r="I57" s="19"/>
+        <v>97.8539816339745</v>
+      </c>
+      <c r="I57" s="30"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G58" s="35" t="s">
-        <v>80</v>
-      </c>
-      <c r="H58" s="36" t="n">
+      <c r="G58" s="48" t="s">
+        <v>81</v>
+      </c>
+      <c r="H58" s="49" t="n">
         <f aca="false">H57+E$49</f>
-        <v>91.7809724509617</v>
-      </c>
-      <c r="I58" s="19"/>
+        <v>101.780972450962</v>
+      </c>
+      <c r="I58" s="30"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G59" s="1" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H59" s="8" t="n">
         <f aca="false">H58+E$49</f>
-        <v>95.707963267949</v>
-      </c>
-      <c r="I59" s="19"/>
+        <v>105.707963267949</v>
+      </c>
+      <c r="I59" s="30"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G60" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="H60" s="36" t="n">
+      <c r="G60" s="48" t="s">
+        <v>83</v>
+      </c>
+      <c r="H60" s="49" t="n">
         <f aca="false">H59+$D$47/2-E$46</f>
-        <v>105.707963267949</v>
-      </c>
-      <c r="I60" s="19"/>
+        <v>115.707963267949</v>
+      </c>
+      <c r="I60" s="30"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H61" s="8"/>
-      <c r="I61" s="19"/>
+      <c r="I61" s="30"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G62" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H62" s="8" t="n">
         <f aca="false">2*($D$47+$D$48)-E$52</f>
-        <v>105.707963267949</v>
-      </c>
-      <c r="I62" s="19"/>
+        <v>115.707963267949</v>
+      </c>
+      <c r="I62" s="30"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H63" s="19"/>
-      <c r="I63" s="19"/>
+      <c r="H63" s="30"/>
+      <c r="I63" s="30"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E64" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F64" s="13"/>
-      <c r="H64" s="19"/>
-      <c r="I64" s="19"/>
+      <c r="E64" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="F64" s="24"/>
+      <c r="H64" s="30"/>
+      <c r="I64" s="30"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E65" s="37" t="s">
+      <c r="E65" s="50" t="s">
         <v>15</v>
       </c>
-      <c r="F65" s="38" t="s">
+      <c r="F65" s="51" t="s">
         <v>18</v>
       </c>
-      <c r="G65" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="H65" s="19"/>
-      <c r="I65" s="19"/>
+      <c r="G65" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="H65" s="30"/>
+      <c r="I65" s="30"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D66" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="E66" s="30" t="n">
+        <v>87</v>
+      </c>
+      <c r="E66" s="53" t="n">
         <f aca="false">2+D47</f>
         <v>32</v>
       </c>
-      <c r="F66" s="31" t="n">
+      <c r="F66" s="54" t="n">
         <f aca="false">2+D48</f>
-        <v>29.1460183660255</v>
-      </c>
-      <c r="G66" s="32" t="n">
+        <v>34.1460183660255</v>
+      </c>
+      <c r="G66" s="55" t="n">
         <f aca="false">SQRT(E66*E66+F66*F66)</f>
-        <v>43.2838351650209</v>
+        <v>46.7969076996862</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C67" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -2774,15 +2991,91 @@
     <mergeCell ref="B42:C42"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+  <pageMargins left="0.7875" right="0.7875" top="0.886111111111111" bottom="0.886111111111111" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="true" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CSeite &amp;P</oddFooter>
+    <firstHeader/>
+    <firstFooter/>
   </headerFooter>
   <drawing r:id="rId1"/>
   <tableParts>
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
+  </sheetPr>
+  <dimension ref="B5:D9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.37"/>
+  </cols>
+  <sheetData>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="56" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="56" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="57" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="58" t="n">
+        <v>12</v>
+      </c>
+      <c r="D6" s="59" t="n">
+        <f aca="false">C6/2-1</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="57" t="s">
+        <v>93</v>
+      </c>
+      <c r="C7" s="58" t="n">
+        <v>30.48</v>
+      </c>
+      <c r="D7" s="59" t="n">
+        <f aca="false">C7/2-1</f>
+        <v>14.24</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="57"/>
+      <c r="C8" s="60"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="57"/>
+      <c r="C9" s="60"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.886111111111111" bottom="0.886111111111111" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="true" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CSeite &amp;P</oddFooter>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
baglabs: correct volumen, text for XLS file
</commit_message>
<xml_diff>
--- a/static/files/Baglab_roundedCorners.xlsx
+++ b/static/files/Baglab_roundedCorners.xlsx
@@ -3,24 +3,30 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection lockWindows="false"/>
+  <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Double U" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Cut Du" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Radius helper" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Cut Out" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Radius helper" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'Cut Du'!$A$1:$N$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm.Print_Area" vbProcedure="false">'Cut Out'!$A$1:$Q$43</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Double U'!$A$1:$Q$43</definedName>
     <definedName function="false" hidden="false" name="Br" vbProcedure="false">'Double U'!$C$7</definedName>
-    <definedName function="false" hidden="false" name="Ho" vbProcedure="false">'Double U'!$C$8</definedName>
     <definedName function="false" hidden="false" name="Hs" vbProcedure="false">'Double U'!$C$9</definedName>
     <definedName function="false" hidden="false" name="L" vbProcedure="false">'Double U'!$C$6</definedName>
     <definedName function="false" hidden="false" name="Rb" vbProcedure="false">'Double U'!$E$5</definedName>
     <definedName function="false" hidden="false" name="Rt" vbProcedure="false">'Double U'!$D$5</definedName>
+    <definedName function="false" hidden="false" name="t" vbProcedure="false">'Double U'!$C$8</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="Hco" vbProcedure="false">'Cut Out'!$C$7</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="Lco" vbProcedure="false">'Cut Out'!$C$6</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="rco" vbProcedure="false">'Cut Out'!$C$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="tco" vbProcedure="false">'Cut Out'!$C$8</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -32,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="101">
   <si>
     <t xml:space="preserve">ROUND</t>
   </si>
@@ -299,6 +305,27 @@
   </si>
   <si>
     <t xml:space="preserve">siehe obrn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aufsetztasche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">höhe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tiefe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only relevant for dimension Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R/2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">halg</t>
   </si>
   <si>
     <t xml:space="preserve">What </t>
@@ -476,7 +503,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -610,6 +637,27 @@
       <bottom style="double"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -635,42 +683,44 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="59">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -678,7 +728,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -698,43 +748,39 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -742,23 +788,23 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="8" fillId="6" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -774,11 +820,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -806,10 +848,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="15" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -822,19 +860,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="166" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -850,39 +884,43 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="18" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="10" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="11" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="12" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="11" fillId="13" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="12" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="13" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="11" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="12" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="13" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="12" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -898,6 +936,10 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
+      <font>
+        <name val="Arial"/>
+        <family val="2"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -1014,9 +1056,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>668160</xdr:colOff>
+      <xdr:colOff>667800</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>110520</xdr:rowOff>
+      <xdr:rowOff>110160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1029,8 +1071,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7702920" y="373320"/>
-          <a:ext cx="6310440" cy="6616800"/>
+          <a:off x="7702560" y="373320"/>
+          <a:ext cx="6309720" cy="6616440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1056,9 +1098,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>339840</xdr:colOff>
+      <xdr:colOff>339480</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>131040</xdr:rowOff>
+      <xdr:rowOff>130680</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1072,7 +1114,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7363080" y="6702120"/>
-          <a:ext cx="3224520" cy="4203720"/>
+          <a:ext cx="3224160" cy="4203360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1093,9 +1135,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>643680</xdr:colOff>
+      <xdr:colOff>643320</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>147960</xdr:rowOff>
+      <xdr:rowOff>147600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1109,7 +1151,49 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4579920" y="289440"/>
-          <a:ext cx="6311520" cy="6616080"/>
+          <a:ext cx="6311160" cy="6615720"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="0">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1122840</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>26280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>306000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>61920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Bild 3" descr=""/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3564360" y="1578240"/>
+          <a:ext cx="3583800" cy="2028240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1153,8 +1237,8 @@
   </sheetPr>
   <dimension ref="A1:K73"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1298,8 +1382,8 @@
         <v>21</v>
       </c>
       <c r="C10" s="9" t="n">
-        <f aca="false">(L*Br*Ho)/1000-( (4-PI()) *(L*Rb + Br*Rt  )/200)</f>
-        <v>42.5106186954104</v>
+        <f aca="false">(L*Br*t)/1000-( (4-PI()) *(L*Rb*Rb + Br*Rt*Rt  )/2000)</f>
+        <v>42.9054860747591</v>
       </c>
       <c r="D10" s="10"/>
     </row>
@@ -1354,7 +1438,7 @@
         <v>22</v>
       </c>
       <c r="C14" s="16" t="n">
-        <f aca="false">2+L+2*Ho -2*Hs-Rt*(4-PI())</f>
+        <f aca="false">2+L+2*t -2*Hs-Rt*(4-PI())</f>
         <v>62.5575191894877</v>
       </c>
       <c r="D14" s="17" t="n">
@@ -1369,7 +1453,7 @@
         <v>22</v>
       </c>
       <c r="H14" s="16" t="n">
-        <f aca="false">2+L+2*(Ho-Hs)</f>
+        <f aca="false">2+L+2*(t-Hs)</f>
         <v>72</v>
       </c>
       <c r="I14" s="17" t="n">
@@ -1385,12 +1469,12 @@
         <f aca="false">2+Br</f>
         <v>32</v>
       </c>
-      <c r="C15" s="19" t="n">
+      <c r="C15" s="8" t="n">
         <f aca="false">2+Br</f>
         <v>32</v>
       </c>
-      <c r="D15" s="20" t="n">
-        <f aca="false">2+2*(Ho)+Br-Rb*(4-PI())</f>
+      <c r="D15" s="19" t="n">
+        <f aca="false">2+2*(t)+Br-Rb*(4-PI())</f>
         <v>87.707963267949</v>
       </c>
       <c r="F15" s="14" t="s">
@@ -1400,12 +1484,12 @@
         <f aca="false">2+Br</f>
         <v>32</v>
       </c>
-      <c r="H15" s="19" t="n">
+      <c r="H15" s="8" t="n">
         <f aca="false">2+Br</f>
         <v>32</v>
       </c>
-      <c r="I15" s="20" t="n">
-        <f aca="false">2+2*(Ho)+Br</f>
+      <c r="I15" s="19" t="n">
+        <f aca="false">2+2*(t)+Br</f>
         <v>92</v>
       </c>
     </row>
@@ -1413,30 +1497,30 @@
       <c r="A16" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B16" s="21" t="n">
+      <c r="B16" s="20" t="n">
         <f aca="false">SQRT(B14*B14+B15*B15)</f>
         <v>38.8329756778952</v>
       </c>
-      <c r="C16" s="22" t="n">
+      <c r="C16" s="21" t="n">
         <f aca="false">SQRT(C14*C14+C15*C15)</f>
         <v>70.26694249178</v>
       </c>
-      <c r="D16" s="23" t="n">
+      <c r="D16" s="22" t="n">
         <f aca="false">SQRT(D14*D14+D15*D15)</f>
         <v>101.964144779486</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="21" t="n">
+      <c r="G16" s="20" t="n">
         <f aca="false">SQRT(G14*G14+G15*G15)</f>
         <v>38.8329756778952</v>
       </c>
-      <c r="H16" s="22" t="n">
+      <c r="H16" s="21" t="n">
         <f aca="false">SQRT(H14*H14+H15*H15)</f>
         <v>78.7908624143688</v>
       </c>
-      <c r="I16" s="23" t="n">
+      <c r="I16" s="22" t="n">
         <f aca="false">SQRT(I14*I14+I15*I15)</f>
         <v>105.678758508983</v>
       </c>
@@ -1461,33 +1545,33 @@
         <v>33</v>
       </c>
       <c r="G19" s="14"/>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="I19" s="24" t="s">
+      <c r="I19" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="25" t="s">
+      <c r="B20" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="26" t="n">
+      <c r="C20" s="25" t="n">
         <v>0</v>
       </c>
-      <c r="D20" s="26" t="n">
+      <c r="D20" s="25" t="n">
         <v>0</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G20" s="25" t="s">
+      <c r="G20" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="H20" s="27" t="n">
+      <c r="H20" s="26" t="n">
         <v>0</v>
       </c>
-      <c r="I20" s="27" t="n">
+      <c r="I20" s="26" t="n">
         <v>0</v>
       </c>
       <c r="J20" s="1" t="s">
@@ -1495,38 +1579,38 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="25"/>
-      <c r="C21" s="26" t="n">
+      <c r="B21" s="24"/>
+      <c r="C21" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="26" t="n">
+      <c r="D21" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="G21" s="25"/>
-      <c r="H21" s="27" t="n">
+      <c r="G21" s="24"/>
+      <c r="H21" s="26" t="n">
         <v>1</v>
       </c>
-      <c r="I21" s="27" t="n">
+      <c r="I21" s="26" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="25"/>
-      <c r="C22" s="28" t="n">
+      <c r="B22" s="24"/>
+      <c r="C22" s="27" t="n">
         <f aca="false">C21+E5</f>
         <v>6</v>
       </c>
-      <c r="D22" s="28" t="n">
+      <c r="D22" s="27" t="n">
         <f aca="false">D21+D5</f>
         <v>12</v>
       </c>
-      <c r="G22" s="25"/>
-      <c r="H22" s="27" t="n">
-        <f aca="false">H21+(Ho -Hs)</f>
+      <c r="G22" s="24"/>
+      <c r="H22" s="26" t="n">
+        <f aca="false">H21+(t -Hs)</f>
         <v>11</v>
       </c>
-      <c r="I22" s="27" t="n">
-        <f aca="false">I21+(Ho)</f>
+      <c r="I22" s="26" t="n">
+        <f aca="false">I21+(t)</f>
         <v>31</v>
       </c>
       <c r="J22" s="1" t="s">
@@ -1534,103 +1618,103 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="25"/>
-      <c r="C23" s="28" t="n">
+      <c r="B23" s="24"/>
+      <c r="C23" s="27" t="n">
         <f aca="false">C24-$D$11</f>
         <v>20</v>
       </c>
-      <c r="D23" s="28" t="n">
+      <c r="D23" s="27" t="n">
         <f aca="false">D24-$E$11</f>
         <v>26</v>
       </c>
-      <c r="G23" s="25" t="s">
+      <c r="G23" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="H23" s="29" t="n">
+      <c r="H23" s="28" t="n">
         <f aca="false">H22+L/2</f>
         <v>36</v>
       </c>
-      <c r="I23" s="29" t="n">
+      <c r="I23" s="28" t="n">
         <f aca="false">I22+Br / 2</f>
         <v>46</v>
       </c>
-      <c r="J23" s="30" t="s">
+      <c r="J23" s="29" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C24" s="26" t="n">
-        <f aca="false">C21+Ho-Rt*(1-PI()/4)</f>
+      <c r="C24" s="25" t="n">
+        <f aca="false">C21+t-Rt*(1-PI()/4)</f>
         <v>28.6393797973719</v>
       </c>
-      <c r="D24" s="26" t="n">
-        <f aca="false">D21+Ho-Rb*(1-PI()/4)</f>
+      <c r="D24" s="25" t="n">
+        <f aca="false">D21+t-Rb*(1-PI()/4)</f>
         <v>29.9269908169872</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="G24" s="25" t="s">
+      <c r="G24" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="27" t="n">
+      <c r="H24" s="26" t="n">
         <f aca="false">H22+L</f>
         <v>61</v>
       </c>
-      <c r="I24" s="27" t="n">
+      <c r="I24" s="26" t="n">
         <f aca="false">I22+Br</f>
         <v>61</v>
       </c>
-      <c r="J24" s="30" t="s">
+      <c r="J24" s="29" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="25"/>
-      <c r="C25" s="28" t="n">
+      <c r="B25" s="24"/>
+      <c r="C25" s="27" t="n">
         <f aca="false">C24+$D$11</f>
         <v>37.2787595947439</v>
       </c>
-      <c r="D25" s="28" t="n">
+      <c r="D25" s="27" t="n">
         <f aca="false">D24+$E$11</f>
         <v>33.8539816339745</v>
       </c>
-      <c r="G25" s="25"/>
-      <c r="H25" s="27" t="n">
-        <f aca="false">H24+(Ho -Hs)</f>
+      <c r="G25" s="24"/>
+      <c r="H25" s="26" t="n">
+        <f aca="false">H24+(t -Hs)</f>
         <v>71</v>
       </c>
-      <c r="I25" s="27" t="n">
-        <f aca="false">I24+(Ho)</f>
+      <c r="I25" s="26" t="n">
+        <f aca="false">I24+(t)</f>
         <v>91</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="25" t="s">
+      <c r="B26" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C26" s="26" t="n">
+      <c r="C26" s="25" t="n">
         <f aca="false">C24+L/2-Rt*(1-PI()/4)</f>
         <v>51.2787595947439</v>
       </c>
-      <c r="D26" s="26" t="n">
+      <c r="D26" s="25" t="n">
         <f aca="false">D24+Br/2-Rb*(1-PI()/4)</f>
         <v>43.8539816339745</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="G26" s="25" t="s">
+      <c r="G26" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="H26" s="27" t="n">
+      <c r="H26" s="26" t="n">
         <f aca="false">H25+1</f>
         <v>72</v>
       </c>
-      <c r="I26" s="27" t="n">
+      <c r="I26" s="26" t="n">
         <f aca="false">I25+1</f>
         <v>92</v>
       </c>
@@ -1639,50 +1723,50 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="25"/>
-      <c r="C27" s="28" t="n">
+      <c r="B27" s="24"/>
+      <c r="C27" s="27" t="n">
         <f aca="false">C28-$D$11</f>
         <v>65.2787595947439</v>
       </c>
-      <c r="D27" s="28" t="n">
+      <c r="D27" s="27" t="n">
         <f aca="false">D28-$E$11</f>
         <v>53.8539816339745</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="25" t="s">
+      <c r="B28" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="26" t="n">
+      <c r="C28" s="25" t="n">
         <f aca="false">C26+L/2-Rt*(1-PI()/4)</f>
         <v>73.9181393921158</v>
       </c>
-      <c r="D28" s="26" t="n">
+      <c r="D28" s="25" t="n">
         <f aca="false">D26+Br/2-Rb*(1-PI()/4)</f>
         <v>57.7809724509617</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="29" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="25"/>
-      <c r="C29" s="28" t="n">
+      <c r="B29" s="24"/>
+      <c r="C29" s="27" t="n">
         <f aca="false">C28+$D$11</f>
         <v>82.5575191894877</v>
       </c>
-      <c r="D29" s="28" t="n">
+      <c r="D29" s="27" t="n">
         <f aca="false">D28+$E$11</f>
         <v>61.707963267949</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="25"/>
-      <c r="C30" s="28" t="n">
+      <c r="B30" s="24"/>
+      <c r="C30" s="27" t="n">
         <f aca="false">C31-$E$5</f>
         <v>96.5575191894877</v>
       </c>
-      <c r="D30" s="28" t="n">
+      <c r="D30" s="27" t="n">
         <f aca="false">D31-$D$5</f>
         <v>75.707963267949</v>
       </c>
@@ -1691,46 +1775,46 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="25"/>
-      <c r="C31" s="26" t="n">
-        <f aca="false">C28+Ho-Rt*(1-PI()/4)</f>
+      <c r="B31" s="24"/>
+      <c r="C31" s="25" t="n">
+        <f aca="false">C28+t-Rt*(1-PI()/4)</f>
         <v>101.557519189488</v>
       </c>
-      <c r="D31" s="26" t="n">
-        <f aca="false">D28+Ho-Rb*(1-PI()/4)</f>
+      <c r="D31" s="25" t="n">
+        <f aca="false">D28+t-Rb*(1-PI()/4)</f>
         <v>86.707963267949</v>
       </c>
-      <c r="E31" s="30"/>
+      <c r="E31" s="29"/>
       <c r="F31" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="25" t="s">
+      <c r="B32" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="26" t="n">
+      <c r="C32" s="25" t="n">
         <f aca="false">C31+1</f>
         <v>102.557519189488</v>
       </c>
-      <c r="D32" s="26" t="n">
+      <c r="D32" s="25" t="n">
         <f aca="false">D31+1</f>
         <v>87.707963267949</v>
       </c>
-      <c r="E32" s="30" t="s">
+      <c r="E32" s="29" t="s">
         <v>43</v>
       </c>
       <c r="G32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="25"/>
+      <c r="B33" s="24"/>
       <c r="G33" s="8"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="25"/>
+      <c r="B34" s="24"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="25"/>
+      <c r="B35" s="24"/>
       <c r="C35" s="12" t="s">
         <v>47</v>
       </c>
@@ -1739,13 +1823,13 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="25" t="s">
+      <c r="B36" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="28" t="n">
+      <c r="C36" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="D36" s="28" t="n">
+      <c r="D36" s="27" t="n">
         <v>0</v>
       </c>
       <c r="E36" s="1" t="s">
@@ -1753,34 +1837,34 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="25"/>
-      <c r="C37" s="28" t="n">
+      <c r="B37" s="24"/>
+      <c r="C37" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="D37" s="28" t="n">
+      <c r="D37" s="27" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="25"/>
-      <c r="C38" s="28" t="n">
+      <c r="B38" s="24"/>
+      <c r="C38" s="27" t="n">
         <f aca="false">C37+$E$5</f>
         <v>6</v>
       </c>
-      <c r="D38" s="28" t="n">
+      <c r="D38" s="27" t="n">
         <f aca="false">D37+$D$5</f>
         <v>12</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="25" t="n">
+      <c r="B39" s="24" t="n">
         <v>9.3</v>
       </c>
-      <c r="C39" s="28" t="n">
+      <c r="C39" s="27" t="n">
         <f aca="false">C37+Br/2</f>
         <v>16</v>
       </c>
-      <c r="D39" s="28" t="n">
+      <c r="D39" s="27" t="n">
         <f aca="false">D37+L/2</f>
         <v>26</v>
       </c>
@@ -1789,56 +1873,56 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="25"/>
-      <c r="C40" s="28" t="n">
+      <c r="B40" s="24"/>
+      <c r="C40" s="27" t="n">
         <f aca="false">C41-$E$5</f>
         <v>26</v>
       </c>
-      <c r="D40" s="28" t="n">
+      <c r="D40" s="27" t="n">
         <f aca="false">D41-$D$5</f>
         <v>40</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="25"/>
-      <c r="C41" s="28" t="n">
+      <c r="B41" s="24"/>
+      <c r="C41" s="27" t="n">
         <f aca="false">Br + 1</f>
         <v>31</v>
       </c>
-      <c r="D41" s="28" t="n">
+      <c r="D41" s="27" t="n">
         <f aca="false">L + 1</f>
         <v>51</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C42" s="28" t="n">
+      <c r="C42" s="27" t="n">
         <f aca="false">C41+1</f>
         <v>32</v>
       </c>
-      <c r="D42" s="28" t="n">
+      <c r="D42" s="27" t="n">
         <f aca="false">D41+1</f>
         <v>52</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H42" s="19"/>
-      <c r="I42" s="19"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H47" s="19"/>
-      <c r="I47" s="19"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H48" s="19"/>
-      <c r="I48" s="19"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I58" s="19" t="n">
-        <f aca="false">2+L+2*Ho -Rt*(4-PI())</f>
+      <c r="I58" s="8" t="n">
+        <f aca="false">2+L+2*t -Rt*(4-PI())</f>
         <v>102.557519189488</v>
       </c>
     </row>
@@ -2055,7 +2139,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection sheet="true" objects="true" scenarios="true"/>
+  <sheetProtection sheet="true" objects="true" scenarios="true" insertColumns="false" insertRows="false" deleteColumns="false" deleteRows="false"/>
   <mergeCells count="2">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="I1:J1"/>
@@ -2085,8 +2169,8 @@
   </sheetPr>
   <dimension ref="B1:S67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O25" activeCellId="0" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2122,10 +2206,10 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="30" t="s">
         <v>6</v>
       </c>
     </row>
@@ -2133,15 +2217,15 @@
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="24" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="3"/>
-      <c r="E5" s="32" t="n">
+      <c r="E5" s="31" t="n">
         <f aca="false">Rt</f>
         <v>11</v>
       </c>
-      <c r="F5" s="32" t="n">
+      <c r="F5" s="31" t="n">
         <f aca="false">Rb</f>
         <v>5</v>
       </c>
@@ -2154,11 +2238,11 @@
       <c r="I5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="33" t="n">
+      <c r="J5" s="32" t="n">
         <f aca="false">$E$5*(2-PI()/2)</f>
         <v>4.72124040525614</v>
       </c>
-      <c r="K5" s="33" t="n">
+      <c r="K5" s="32" t="n">
         <f aca="false">$F$5*(2-PI()/2)</f>
         <v>2.14601836602552</v>
       </c>
@@ -2170,10 +2254,10 @@
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="31" t="s">
+      <c r="C6" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="32" t="n">
+      <c r="D6" s="31" t="n">
         <f aca="false">L</f>
         <v>50</v>
       </c>
@@ -2183,11 +2267,11 @@
         <v>14</v>
       </c>
       <c r="I6" s="5"/>
-      <c r="J6" s="33" t="n">
+      <c r="J6" s="32" t="n">
         <f aca="false">J5*2</f>
         <v>9.44248081051228</v>
       </c>
-      <c r="K6" s="33" t="n">
+      <c r="K6" s="32" t="n">
         <f aca="false">K5*2</f>
         <v>4.29203673205103</v>
       </c>
@@ -2199,25 +2283,25 @@
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="32" t="n">
+      <c r="D7" s="31" t="n">
         <f aca="false">Br</f>
         <v>30</v>
       </c>
-      <c r="E7" s="34" t="s">
+      <c r="E7" s="33" t="s">
         <v>50</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>17</v>
       </c>
       <c r="I7" s="5"/>
-      <c r="J7" s="33" t="n">
+      <c r="J7" s="32" t="n">
         <f aca="false">J6*2</f>
         <v>18.8849616210246</v>
       </c>
-      <c r="K7" s="33" t="n">
+      <c r="K7" s="32" t="n">
         <f aca="false">K6*2</f>
         <v>8.58407346410207</v>
       </c>
@@ -2238,14 +2322,14 @@
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="32" t="n">
-        <f aca="false"> Ho</f>
+      <c r="D8" s="31" t="n">
+        <f aca="false">t</f>
         <v>30</v>
       </c>
-      <c r="E8" s="34" t="s">
+      <c r="E8" s="33" t="s">
         <v>55</v>
       </c>
       <c r="H8" s="5" t="s">
@@ -2254,24 +2338,24 @@
       <c r="I8" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="33" t="n">
+      <c r="J8" s="32" t="n">
         <f aca="false">PI()/4*E5</f>
         <v>8.63937979737193</v>
       </c>
-      <c r="K8" s="33" t="n">
+      <c r="K8" s="32" t="n">
         <f aca="false">PI()/4*F5</f>
         <v>3.92699081698724</v>
       </c>
       <c r="Q8" s="8" t="n">
         <v>40</v>
       </c>
-      <c r="R8" s="35" t="n">
+      <c r="R8" s="3" t="n">
         <f aca="false">PI()/4*Q8*Q8</f>
         <v>1256.63706143592</v>
       </c>
       <c r="S8" s="1" t="n">
         <f aca="false">SQRT(R8)</f>
-        <v>35.4490770181103</v>
+        <v>35.4490770181104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2287,13 +2371,13 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="11"/>
-      <c r="C10" s="36" t="s">
+      <c r="C10" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="37" t="s">
+      <c r="D10" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="E10" s="36" t="s">
         <v>57</v>
       </c>
       <c r="R10" s="1" t="n">
@@ -2306,15 +2390,15 @@
       <c r="B11" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="39" t="n">
-        <f aca="false">2+L+Ho -Rt*(4-PI())/2</f>
+      <c r="C11" s="37" t="n">
+        <f aca="false">2+L+t -Rt*(4-PI())/2</f>
         <v>77.2787595947439</v>
       </c>
-      <c r="D11" s="40" t="n">
+      <c r="D11" s="38" t="n">
         <f aca="false">2+L</f>
         <v>52</v>
       </c>
-      <c r="E11" s="41" t="n">
+      <c r="E11" s="39" t="n">
         <f aca="false">G18+2</f>
         <v>34.1460183660255</v>
       </c>
@@ -2323,15 +2407,15 @@
       <c r="B12" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="39" t="n">
+      <c r="C12" s="37" t="n">
         <f aca="false">2+Br</f>
         <v>32</v>
       </c>
-      <c r="D12" s="40" t="n">
-        <f aca="false">2+2*(Ho)+Br-Rb*(4-PI())</f>
+      <c r="D12" s="38" t="n">
+        <f aca="false">2+2*(t)+Br-Rb*(4-PI())</f>
         <v>87.707963267949</v>
       </c>
-      <c r="E12" s="42" t="n">
+      <c r="E12" s="39" t="n">
         <f aca="false">2+Br</f>
         <v>32</v>
       </c>
@@ -2340,15 +2424,15 @@
       <c r="B13" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="43" t="n">
+      <c r="C13" s="40" t="n">
         <f aca="false">SQRT(C11*C11+C12*C12)</f>
         <v>83.6421346242563</v>
       </c>
-      <c r="D13" s="44" t="n">
+      <c r="D13" s="41" t="n">
         <f aca="false">SQRT(D11*D11+D12*D12)</f>
         <v>101.964144779486</v>
       </c>
-      <c r="E13" s="45" t="n">
+      <c r="E13" s="42" t="n">
         <f aca="false">SQRT(E11*E11+E12*E12)</f>
         <v>46.7969076996862</v>
       </c>
@@ -2374,11 +2458,11 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="25" t="s">
+      <c r="B17" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26" t="n">
+      <c r="C17" s="25"/>
+      <c r="D17" s="25" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="1" t="s">
@@ -2393,15 +2477,15 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="25"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26" t="n">
+      <c r="B18" s="24"/>
+      <c r="C18" s="25"/>
+      <c r="D18" s="25" t="n">
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="G18" s="46" t="n">
+      <c r="G18" s="43" t="n">
         <f aca="false">(G17+K7-2*D7)/2</f>
         <v>32.1460183660255</v>
       </c>
@@ -2410,31 +2494,31 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="25"/>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28" t="n">
+      <c r="B19" s="24"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27" t="n">
         <f aca="false">D18+E5</f>
         <v>12</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="25"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28" t="n">
+      <c r="B20" s="24"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27" t="n">
         <f aca="false">D21-$K$8</f>
         <v>26</v>
       </c>
       <c r="G20" s="10"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="26" t="n">
+      <c r="C21" s="25" t="n">
         <v>1</v>
       </c>
-      <c r="D21" s="26" t="n">
-        <f aca="false">D18+Ho-Rb*(1-PI()/4)</f>
+      <c r="D21" s="25" t="n">
+        <f aca="false">D18+t-Rb*(1-PI()/4)</f>
         <v>29.9269908169872</v>
       </c>
       <c r="E21" s="1" t="s">
@@ -2443,109 +2527,109 @@
       <c r="G21" s="10"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="25"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28" t="n">
+      <c r="B22" s="24"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27" t="n">
         <f aca="false">D21+$K$8</f>
         <v>33.8539816339745</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="25" t="s">
+      <c r="B23" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="26" t="n">
+      <c r="C23" s="25" t="n">
         <f aca="false">C21+L/2</f>
         <v>26</v>
       </c>
-      <c r="D23" s="26" t="n">
+      <c r="D23" s="25" t="n">
         <f aca="false">D21+Br/2-Rb*(1-PI()/4)</f>
         <v>43.8539816339745</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="29" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="25"/>
-      <c r="C24" s="28" t="n">
+      <c r="B24" s="24"/>
+      <c r="C24" s="27" t="n">
         <f aca="false">C25-$J$8</f>
         <v>40</v>
       </c>
-      <c r="D24" s="28" t="n">
+      <c r="D24" s="27" t="n">
         <f aca="false">D25-$K$8</f>
         <v>53.8539816339745</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="25" t="s">
+      <c r="B25" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="26" t="n">
+      <c r="C25" s="25" t="n">
         <f aca="false">C23+L/2-Rt*(1-PI()/4)</f>
         <v>48.6393797973719</v>
       </c>
-      <c r="D25" s="26" t="n">
+      <c r="D25" s="25" t="n">
         <f aca="false">D23+Br/2-Rb*(1-PI()/4)</f>
         <v>57.7809724509617</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="29" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="25"/>
-      <c r="C26" s="28" t="n">
+      <c r="B26" s="24"/>
+      <c r="C26" s="27" t="n">
         <f aca="false">C25+$J$8</f>
         <v>57.2787595947439</v>
       </c>
-      <c r="D26" s="28" t="n">
+      <c r="D26" s="27" t="n">
         <f aca="false">D25+$K$8</f>
         <v>61.707963267949</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="25"/>
-      <c r="C27" s="28" t="n">
+      <c r="B27" s="24"/>
+      <c r="C27" s="27" t="n">
         <f aca="false">C28-$F$5</f>
         <v>71.2787595947439</v>
       </c>
-      <c r="D27" s="28" t="n">
+      <c r="D27" s="27" t="n">
         <f aca="false">D28-$E$5</f>
         <v>75.707963267949</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="25"/>
-      <c r="C28" s="26" t="n">
-        <f aca="false">C25+Ho-Rt*(1-PI()/4)</f>
+      <c r="B28" s="24"/>
+      <c r="C28" s="25" t="n">
+        <f aca="false">C25+t-Rt*(1-PI()/4)</f>
         <v>76.2787595947439</v>
       </c>
-      <c r="D28" s="26" t="n">
-        <f aca="false">D25+Ho-Rb*(1-PI()/4)</f>
+      <c r="D28" s="25" t="n">
+        <f aca="false">D25+t-Rb*(1-PI()/4)</f>
         <v>86.707963267949</v>
       </c>
-      <c r="E28" s="30"/>
+      <c r="E28" s="29"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="25" t="s">
+      <c r="B29" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C29" s="26" t="n">
+      <c r="C29" s="25" t="n">
         <f aca="false">C28+1</f>
         <v>77.2787595947439</v>
       </c>
-      <c r="D29" s="26" t="n">
+      <c r="D29" s="25" t="n">
         <f aca="false">D28+1</f>
         <v>87.707963267949</v>
       </c>
-      <c r="E29" s="30" t="s">
+      <c r="E29" s="29" t="s">
         <v>43</v>
       </c>
       <c r="G29" s="8"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="25"/>
+      <c r="B30" s="24"/>
       <c r="C30" s="1" t="s">
         <v>61</v>
       </c>
@@ -2555,13 +2639,13 @@
       <c r="G30" s="8"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="25"/>
+      <c r="B31" s="24"/>
       <c r="E31" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="25"/>
+      <c r="B32" s="24"/>
       <c r="C32" s="12" t="s">
         <v>47</v>
       </c>
@@ -2570,13 +2654,13 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="24" t="s">
         <v>34</v>
       </c>
-      <c r="C33" s="28" t="n">
+      <c r="C33" s="27" t="n">
         <v>0</v>
       </c>
-      <c r="D33" s="28" t="n">
+      <c r="D33" s="27" t="n">
         <v>0</v>
       </c>
       <c r="E33" s="1" t="s">
@@ -2584,31 +2668,31 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="25"/>
-      <c r="C34" s="28" t="n">
+      <c r="B34" s="24"/>
+      <c r="C34" s="27" t="n">
         <v>1</v>
       </c>
-      <c r="D34" s="28" t="n">
+      <c r="D34" s="27" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="25"/>
-      <c r="C35" s="28" t="n">
+      <c r="B35" s="24"/>
+      <c r="C35" s="27" t="n">
         <f aca="false">C34+$F$5</f>
         <v>6</v>
       </c>
-      <c r="D35" s="28"/>
+      <c r="D35" s="27"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="25" t="n">
+      <c r="B36" s="24" t="n">
         <v>9.3</v>
       </c>
-      <c r="C36" s="28" t="n">
+      <c r="C36" s="27" t="n">
         <f aca="false">C34+Br/2</f>
         <v>16</v>
       </c>
-      <c r="D36" s="28" t="n">
+      <c r="D36" s="27" t="n">
         <f aca="false">D34+L/2</f>
         <v>26</v>
       </c>
@@ -2617,44 +2701,44 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="25"/>
-      <c r="C37" s="28" t="n">
+      <c r="B37" s="24"/>
+      <c r="C37" s="27" t="n">
         <f aca="false">C38-$F$5</f>
         <v>26</v>
       </c>
-      <c r="D37" s="28" t="n">
+      <c r="D37" s="27" t="n">
         <f aca="false">D38-$E$5</f>
         <v>40</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="25"/>
-      <c r="C38" s="28" t="n">
+      <c r="B38" s="24"/>
+      <c r="C38" s="27" t="n">
         <f aca="false">Br + 1</f>
         <v>31</v>
       </c>
-      <c r="D38" s="28" t="n">
+      <c r="D38" s="27" t="n">
         <f aca="false">L + 1</f>
         <v>51</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="28" t="n">
+      <c r="C39" s="27" t="n">
         <f aca="false">C38+1</f>
         <v>32</v>
       </c>
-      <c r="D39" s="28" t="n">
+      <c r="D39" s="27" t="n">
         <f aca="false">D38+1</f>
         <v>52</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H39" s="19"/>
-      <c r="I39" s="19"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="1" t="s">
@@ -2666,9 +2750,9 @@
         <v>63</v>
       </c>
       <c r="C42" s="2"/>
-      <c r="G42" s="30"/>
-      <c r="H42" s="30"/>
-      <c r="I42" s="30"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="29"/>
+      <c r="I42" s="29"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G43" s="1" t="s">
@@ -2677,7 +2761,7 @@
       <c r="H43" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I43" s="30"/>
+      <c r="I43" s="29"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C44" s="1" t="s">
@@ -2692,7 +2776,7 @@
       <c r="H44" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="I44" s="47"/>
+      <c r="I44" s="10"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G45" s="1" t="s">
@@ -2702,13 +2786,13 @@
         <f aca="false">$D$47/2-E$46</f>
         <v>10</v>
       </c>
-      <c r="I45" s="47"/>
+      <c r="I45" s="10"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C46" s="31" t="s">
+      <c r="C46" s="30" t="s">
         <v>8</v>
       </c>
       <c r="D46" s="3"/>
@@ -2716,23 +2800,23 @@
         <f aca="false">F5</f>
         <v>5</v>
       </c>
-      <c r="G46" s="48" t="s">
+      <c r="G46" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="H46" s="49" t="n">
+      <c r="H46" s="45" t="n">
         <f aca="false">H45+E$49</f>
         <v>13.9269908169872</v>
       </c>
-      <c r="I46" s="47"/>
+      <c r="I46" s="10"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C47" s="31" t="s">
+      <c r="C47" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="46" t="n">
+      <c r="D47" s="43" t="n">
         <f aca="false">D7</f>
         <v>30</v>
       </c>
@@ -2743,27 +2827,27 @@
         <f aca="false">H46+E$49</f>
         <v>17.8539816339745</v>
       </c>
-      <c r="I47" s="30"/>
+      <c r="I47" s="29"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C48" s="31" t="s">
+      <c r="C48" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="D48" s="46" t="n">
+      <c r="D48" s="43" t="n">
         <f aca="false">G18</f>
         <v>32.1460183660255</v>
       </c>
-      <c r="G48" s="48" t="s">
+      <c r="G48" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="H48" s="49" t="n">
+      <c r="H48" s="45" t="n">
         <f aca="false">H47+$D$48/2-E$46</f>
         <v>28.9269908169872</v>
       </c>
-      <c r="I48" s="30"/>
+      <c r="I48" s="29"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C49" s="1" t="s">
@@ -2783,7 +2867,7 @@
         <f aca="false">H48+$D$48/2-E$46</f>
         <v>40</v>
       </c>
-      <c r="I49" s="30"/>
+      <c r="I49" s="29"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="1" t="s">
@@ -2799,14 +2883,14 @@
         <f aca="false">E$46*(2-PI()/2)</f>
         <v>2.14601836602552</v>
       </c>
-      <c r="G50" s="48" t="s">
+      <c r="G50" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="H50" s="49" t="n">
+      <c r="H50" s="45" t="n">
         <f aca="false">H49+E$49</f>
         <v>43.9269908169872</v>
       </c>
-      <c r="I50" s="30"/>
+      <c r="I50" s="29"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C51" s="1" t="s">
@@ -2823,7 +2907,7 @@
         <f aca="false">H50+E$49</f>
         <v>47.8539816339745</v>
       </c>
-      <c r="I51" s="30"/>
+      <c r="I51" s="29"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C52" s="1" t="s">
@@ -2833,14 +2917,14 @@
         <f aca="false">E51*2</f>
         <v>8.58407346410207</v>
       </c>
-      <c r="G52" s="48" t="s">
+      <c r="G52" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="H52" s="49" t="n">
+      <c r="H52" s="45" t="n">
         <f aca="false">H51+$D$47/2-E$46</f>
         <v>57.8539816339745</v>
       </c>
-      <c r="I52" s="30"/>
+      <c r="I52" s="29"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G53" s="1" t="s">
@@ -2850,17 +2934,17 @@
         <f aca="false">H52+$D$47/2-E$46</f>
         <v>67.8539816339745</v>
       </c>
-      <c r="I53" s="30"/>
+      <c r="I53" s="29"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G54" s="48" t="s">
+      <c r="G54" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="H54" s="49" t="n">
+      <c r="H54" s="45" t="n">
         <f aca="false">H53+E$49</f>
         <v>71.7809724509617</v>
       </c>
-      <c r="I54" s="30"/>
+      <c r="I54" s="29"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G55" s="1" t="s">
@@ -2870,17 +2954,17 @@
         <f aca="false">H54+E$49</f>
         <v>75.707963267949</v>
       </c>
-      <c r="I55" s="30"/>
+      <c r="I55" s="29"/>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G56" s="48" t="s">
+      <c r="G56" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="H56" s="49" t="n">
+      <c r="H56" s="45" t="n">
         <f aca="false">H55+$D$48/2-E$46</f>
         <v>86.7809724509617</v>
       </c>
-      <c r="I56" s="30"/>
+      <c r="I56" s="29"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G57" s="1" t="s">
@@ -2890,17 +2974,17 @@
         <f aca="false">H56+$D$48/2-E$46</f>
         <v>97.8539816339745</v>
       </c>
-      <c r="I57" s="30"/>
+      <c r="I57" s="29"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G58" s="48" t="s">
+      <c r="G58" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="H58" s="49" t="n">
+      <c r="H58" s="45" t="n">
         <f aca="false">H57+E$49</f>
         <v>101.780972450962</v>
       </c>
-      <c r="I58" s="30"/>
+      <c r="I58" s="29"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G59" s="1" t="s">
@@ -2910,21 +2994,21 @@
         <f aca="false">H58+E$49</f>
         <v>105.707963267949</v>
       </c>
-      <c r="I59" s="30"/>
+      <c r="I59" s="29"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G60" s="48" t="s">
+      <c r="G60" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="H60" s="49" t="n">
+      <c r="H60" s="45" t="n">
         <f aca="false">H59+$D$47/2-E$46</f>
         <v>115.707963267949</v>
       </c>
-      <c r="I60" s="30"/>
+      <c r="I60" s="29"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H61" s="8"/>
-      <c r="I61" s="30"/>
+      <c r="I61" s="29"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G62" s="1" t="s">
@@ -2934,46 +3018,46 @@
         <f aca="false">2*($D$47+$D$48)-E$52</f>
         <v>115.707963267949</v>
       </c>
-      <c r="I62" s="30"/>
+      <c r="I62" s="29"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H63" s="30"/>
-      <c r="I63" s="30"/>
+      <c r="H63" s="29"/>
+      <c r="I63" s="29"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E64" s="24" t="s">
+      <c r="E64" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="F64" s="24"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="30"/>
+      <c r="F64" s="23"/>
+      <c r="H64" s="29"/>
+      <c r="I64" s="29"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E65" s="50" t="s">
+      <c r="E65" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="F65" s="51" t="s">
+      <c r="F65" s="47" t="s">
         <v>18</v>
       </c>
-      <c r="G65" s="52" t="s">
+      <c r="G65" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="H65" s="30"/>
-      <c r="I65" s="30"/>
+      <c r="H65" s="29"/>
+      <c r="I65" s="29"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D66" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="E66" s="53" t="n">
+      <c r="E66" s="40" t="n">
         <f aca="false">2+D47</f>
         <v>32</v>
       </c>
-      <c r="F66" s="54" t="n">
+      <c r="F66" s="41" t="n">
         <f aca="false">2+D48</f>
         <v>34.1460183660255</v>
       </c>
-      <c r="G66" s="55" t="n">
+      <c r="G66" s="42" t="n">
         <f aca="false">SQRT(E66*E66+F66*F66)</f>
         <v>46.7969076996862</v>
       </c>
@@ -3011,61 +3095,813 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
+  <dimension ref="A1:K73"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.58"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.31"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="5" style="1" width="11.53"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" s="0"/>
+      <c r="E5" s="0"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>75</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>10</v>
+      </c>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" s="0"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C9" s="0"/>
+    </row>
+    <row r="10" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C10" s="0"/>
+      <c r="D10" s="10"/>
+      <c r="F10" s="0"/>
+      <c r="G10" s="0"/>
+      <c r="H10" s="0"/>
+      <c r="I10" s="0"/>
+      <c r="J10" s="0"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <f aca="false">PI()/4*rco</f>
+        <v>3.92699081698724</v>
+      </c>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+      <c r="G11" s="0"/>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="0"/>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
+      <c r="J12" s="0"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="0"/>
+      <c r="F13" s="0"/>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="0"/>
+      <c r="C14" s="50" t="n">
+        <f aca="false">C30</f>
+        <v>92.707963267949</v>
+      </c>
+      <c r="D14" s="50" t="n">
+        <f aca="false">Lco + 2</f>
+        <v>77</v>
+      </c>
+      <c r="F14" s="0"/>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="0"/>
+      <c r="C15" s="51" t="n">
+        <f aca="false">2+tco</f>
+        <v>27</v>
+      </c>
+      <c r="D15" s="51" t="n">
+        <f aca="false">tco + 2</f>
+        <v>27</v>
+      </c>
+      <c r="F15" s="0"/>
+      <c r="G15" s="0"/>
+      <c r="H15" s="0"/>
+      <c r="I15" s="0"/>
+      <c r="J15" s="0"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="0"/>
+      <c r="C16" s="52" t="n">
+        <f aca="false">SQRT(C14*C14+C15*C15)</f>
+        <v>96.5596523051496</v>
+      </c>
+      <c r="D16" s="52" t="n">
+        <f aca="false">SQRT(D14*D14+D15*D15)</f>
+        <v>81.5965685553014</v>
+      </c>
+      <c r="F16" s="0"/>
+      <c r="G16" s="0"/>
+      <c r="H16" s="0"/>
+      <c r="I16" s="0"/>
+      <c r="J16" s="0"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="0"/>
+      <c r="G17" s="0"/>
+      <c r="H17" s="0"/>
+      <c r="I17" s="0"/>
+      <c r="J17" s="0"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="0"/>
+      <c r="G18" s="0"/>
+      <c r="H18" s="0"/>
+      <c r="I18" s="0"/>
+      <c r="J18" s="0"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="0"/>
+      <c r="H19" s="0"/>
+      <c r="I19" s="0"/>
+      <c r="J19" s="0"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="53" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
+      <c r="G20" s="0"/>
+      <c r="H20" s="0"/>
+      <c r="I20" s="0"/>
+      <c r="J20" s="0"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="24"/>
+      <c r="C21" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0"/>
+      <c r="I21" s="0"/>
+      <c r="J21" s="0"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="24"/>
+      <c r="C22" s="27" t="n">
+        <f aca="false">C21+(Hco-rco)</f>
+        <v>6</v>
+      </c>
+      <c r="D22" s="0"/>
+      <c r="E22" s="0"/>
+      <c r="F22" s="0"/>
+      <c r="G22" s="0"/>
+      <c r="H22" s="0"/>
+      <c r="I22" s="0"/>
+      <c r="J22" s="0"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="27" t="n">
+        <f aca="false">C22+$D$11</f>
+        <v>9.92699081698724</v>
+      </c>
+      <c r="D23" s="0"/>
+      <c r="E23" s="0"/>
+      <c r="F23" s="0"/>
+      <c r="G23" s="0"/>
+      <c r="H23" s="0"/>
+      <c r="I23" s="0"/>
+      <c r="J23" s="0"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="24"/>
+      <c r="C24" s="27" t="n">
+        <f aca="false">C23+$D$11</f>
+        <v>13.8539816339745</v>
+      </c>
+      <c r="D24" s="0"/>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0"/>
+      <c r="G24" s="0"/>
+      <c r="H24" s="0"/>
+      <c r="I24" s="0"/>
+      <c r="J24" s="0"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="24" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="27" t="n">
+        <f aca="false">C24-rco + Lco/2</f>
+        <v>46.3539816339745</v>
+      </c>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+      <c r="G25" s="0"/>
+      <c r="H25" s="0"/>
+      <c r="I25" s="0"/>
+      <c r="J25" s="0"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="24"/>
+      <c r="C26" s="27" t="n">
+        <f aca="false">C25-rco + Lco/2</f>
+        <v>78.8539816339745</v>
+      </c>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+      <c r="G26" s="0"/>
+      <c r="H26" s="0"/>
+      <c r="I26" s="0"/>
+      <c r="J26" s="0"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="24"/>
+      <c r="C27" s="27" t="n">
+        <f aca="false">C26+$D$11</f>
+        <v>82.7809724509617</v>
+      </c>
+      <c r="D27" s="0"/>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0"/>
+      <c r="G27" s="0"/>
+      <c r="H27" s="0"/>
+      <c r="I27" s="0"/>
+      <c r="J27" s="0"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="27" t="n">
+        <f aca="false">C27+$D$11</f>
+        <v>86.707963267949</v>
+      </c>
+      <c r="D28" s="0"/>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+      <c r="G28" s="0"/>
+      <c r="H28" s="0"/>
+      <c r="I28" s="0"/>
+      <c r="J28" s="0"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="24"/>
+      <c r="C29" s="27" t="n">
+        <f aca="false">C28+(Hco-rco)</f>
+        <v>91.707963267949</v>
+      </c>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="G29" s="0"/>
+      <c r="H29" s="0"/>
+      <c r="I29" s="0"/>
+      <c r="J29" s="0"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="C30" s="27" t="n">
+        <f aca="false">C29+1</f>
+        <v>92.707963267949</v>
+      </c>
+      <c r="D30" s="0"/>
+      <c r="E30" s="0"/>
+      <c r="F30" s="0"/>
+      <c r="G30" s="0"/>
+      <c r="H30" s="0"/>
+      <c r="I30" s="0"/>
+      <c r="J30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="24"/>
+      <c r="C31" s="0"/>
+      <c r="D31" s="0"/>
+      <c r="E31" s="0"/>
+      <c r="F31" s="0"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
+      <c r="G32" s="8"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="24"/>
+      <c r="D33" s="0"/>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
+      <c r="G33" s="8"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0"/>
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0"/>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0"/>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
+      <c r="D39" s="0"/>
+      <c r="E39" s="0"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0"/>
+      <c r="B40" s="0"/>
+      <c r="C40" s="0"/>
+      <c r="D40" s="0"/>
+      <c r="E40" s="0"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0"/>
+      <c r="B41" s="0"/>
+      <c r="C41" s="0"/>
+      <c r="D41" s="0"/>
+      <c r="E41" s="0"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0"/>
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0"/>
+      <c r="B43" s="0"/>
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
+      <c r="E43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0"/>
+      <c r="B44" s="0"/>
+      <c r="C44" s="0"/>
+      <c r="D44" s="0"/>
+      <c r="E44" s="0"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0"/>
+      <c r="B45" s="0"/>
+      <c r="C45" s="0"/>
+      <c r="D45" s="0"/>
+      <c r="E45" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I58" s="8" t="e">
+        <f aca="false">2+L+2*ho -Rt*(4-PI())</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F61" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="G61" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1" t="n">
+        <f aca="false">$G$73 - G61</f>
+        <v>103.845130209103</v>
+      </c>
+      <c r="I61" s="1" t="n">
+        <f aca="false">H61+G61</f>
+        <v>103.845130209103</v>
+      </c>
+      <c r="J61" s="1" t="n">
+        <f aca="false">(60.6-18)/2</f>
+        <v>21.3</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F62" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H62" s="1" t="n">
+        <f aca="false">$G$73 - G62</f>
+        <v>102.845130209103</v>
+      </c>
+      <c r="I62" s="1" t="n">
+        <f aca="false">H62+G62</f>
+        <v>103.845130209103</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F63" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="G63" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="H63" s="1" t="n">
+        <f aca="false">$G$73 - G63</f>
+        <v>97.845130209103</v>
+      </c>
+      <c r="I63" s="1" t="n">
+        <f aca="false">H63+G63</f>
+        <v>103.845130209103</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F64" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="G64" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="H64" s="1" t="n">
+        <f aca="false">$G$73 - G64</f>
+        <v>83.845130209103</v>
+      </c>
+      <c r="I64" s="1" t="n">
+        <f aca="false">H64+G64</f>
+        <v>103.845130209103</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F65" s="1" t="n">
+        <v>28.6393797973719</v>
+      </c>
+      <c r="G65" s="1" t="n">
+        <v>28.6393797973719</v>
+      </c>
+      <c r="H65" s="1" t="n">
+        <f aca="false">$G$73 - G65</f>
+        <v>75.2057504117311</v>
+      </c>
+      <c r="I65" s="1" t="n">
+        <f aca="false">H65+G65</f>
+        <v>103.845130209103</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F66" s="1" t="n">
+        <v>37.2787595947439</v>
+      </c>
+      <c r="G66" s="1" t="n">
+        <v>37.2787595947439</v>
+      </c>
+      <c r="H66" s="1" t="n">
+        <f aca="false">$G$73 - G66</f>
+        <v>66.5663706143591</v>
+      </c>
+      <c r="I66" s="1" t="n">
+        <f aca="false">H66+G66</f>
+        <v>103.845130209103</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F67" s="1" t="n">
+        <v>51.2787595947439</v>
+      </c>
+      <c r="G67" s="1" t="n">
+        <v>51.2787595947439</v>
+      </c>
+      <c r="H67" s="1" t="n">
+        <f aca="false">$G$73 - G67</f>
+        <v>52.5663706143591</v>
+      </c>
+      <c r="I67" s="1" t="n">
+        <f aca="false">H67+G67</f>
+        <v>103.845130209103</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F68" s="1" t="n">
+        <v>65.2787595947439</v>
+      </c>
+      <c r="G68" s="1" t="n">
+        <v>65.2787595947439</v>
+      </c>
+      <c r="H68" s="1" t="n">
+        <f aca="false">$G$73 - G68</f>
+        <v>38.5663706143591</v>
+      </c>
+      <c r="I68" s="1" t="n">
+        <f aca="false">H68+G68</f>
+        <v>103.845130209103</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F69" s="1" t="n">
+        <v>73.9181393921158</v>
+      </c>
+      <c r="G69" s="1" t="n">
+        <v>73.9181393921158</v>
+      </c>
+      <c r="H69" s="1" t="n">
+        <f aca="false">$G$73 - G69</f>
+        <v>29.9269908169872</v>
+      </c>
+      <c r="I69" s="1" t="n">
+        <f aca="false">H69+G69</f>
+        <v>103.845130209103</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F70" s="1" t="n">
+        <v>82.5575191894877</v>
+      </c>
+      <c r="G70" s="1" t="n">
+        <v>82.5575191894877</v>
+      </c>
+      <c r="H70" s="1" t="n">
+        <f aca="false">$G$73 - G70</f>
+        <v>21.2876110196153</v>
+      </c>
+      <c r="I70" s="1" t="n">
+        <f aca="false">H70+G70</f>
+        <v>103.845130209103</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F71" s="1" t="n">
+        <v>97.845130209103</v>
+      </c>
+      <c r="G71" s="1" t="n">
+        <v>97.845130209103</v>
+      </c>
+      <c r="H71" s="1" t="n">
+        <f aca="false">$G$73 - G71</f>
+        <v>6</v>
+      </c>
+      <c r="I71" s="1" t="n">
+        <f aca="false">H71+G71</f>
+        <v>103.845130209103</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F72" s="1" t="n">
+        <v>102.845130209103</v>
+      </c>
+      <c r="G72" s="1" t="n">
+        <v>102.845130209103</v>
+      </c>
+      <c r="H72" s="1" t="n">
+        <f aca="false">$G$73 - G72</f>
+        <v>1</v>
+      </c>
+      <c r="I72" s="1" t="n">
+        <f aca="false">H72+G72</f>
+        <v>103.845130209103</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F73" s="1" t="n">
+        <v>103.845130209103</v>
+      </c>
+      <c r="G73" s="1" t="n">
+        <v>103.845130209103</v>
+      </c>
+      <c r="H73" s="1" t="n">
+        <f aca="false">$G$73 - G73</f>
+        <v>0</v>
+      </c>
+      <c r="I73" s="1" t="n">
+        <f aca="false">H73+G73</f>
+        <v>103.845130209103</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="true" objects="true" scenarios="true"/>
+  <mergeCells count="2">
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="I1:J1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="0.886111111111111" bottom="0.886111111111111" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="true" differentOddEven="false">
+    <oddHeader>&amp;C&amp;A</oddHeader>
+    <oddFooter>&amp;CSeite &amp;P</oddFooter>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="true"/>
+  </sheetPr>
   <dimension ref="B5:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H19" activeCellId="0" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="8.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.37"/>
   </cols>
   <sheetData>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="56" t="s">
-        <v>89</v>
-      </c>
-      <c r="C5" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="56" t="s">
-        <v>91</v>
+      <c r="B5" s="54" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="54" t="s">
+        <v>97</v>
+      </c>
+      <c r="D5" s="54" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="57" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="58" t="n">
+      <c r="B6" s="55" t="s">
+        <v>99</v>
+      </c>
+      <c r="C6" s="56" t="n">
         <v>12</v>
       </c>
-      <c r="D6" s="59" t="n">
+      <c r="D6" s="57" t="n">
         <f aca="false">C6/2-1</f>
         <v>5</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="57" t="s">
-        <v>93</v>
-      </c>
-      <c r="C7" s="58" t="n">
+      <c r="B7" s="55" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="56" t="n">
         <v>30.48</v>
       </c>
-      <c r="D7" s="59" t="n">
+      <c r="D7" s="57" t="n">
         <f aca="false">C7/2-1</f>
         <v>14.24</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="57"/>
-      <c r="C8" s="60"/>
+      <c r="B8" s="55"/>
+      <c r="C8" s="58"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="57"/>
-      <c r="C9" s="60"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="58"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>